<commit_message>
added a ImagingMethod column
</commit_message>
<xml_diff>
--- a/config/becExpConfig/becExpType.csv.xlsx
+++ b/config/becExpConfig/becExpType.csv.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoc\Documents\MMUser\config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weld Lab User\Documents\MMUser\config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F738E4-6FBA-415D-9522-31CB4034DDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46D3F54-A980-4C14-B806-5128AF261ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="1000">
   <si>
     <t>TrialName</t>
   </si>
@@ -2825,45 +2825,6 @@
     <t>StdErr</t>
   </si>
   <si>
-    <t>NiLatticeXvLatticeBm</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting lattice stage. Scan xvlattice. With band mapping.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>BMPDloopTof4000</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>hw_XvLattice</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
     <t>ScopeValueName</t>
   </si>
   <si>
@@ -2958,7 +2919,7 @@
     <t>ODT</t>
   </si>
   <si>
-    <t>NiLattice</t>
+    <t>SideOdtCamera</t>
   </si>
   <si>
     <t>None</t>
@@ -2976,228 +2937,117 @@
     <t>HF</t>
   </si>
   <si>
+    <t>TwoLevelWeakLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>NiBecSlosh</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting BEC stage. Snapping both ODT and XODT off then on.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>NiSloshTime</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
     <t>StrongLight</t>
   </si>
   <si>
     <t>BosonicGaussianFit1D</t>
   </si>
   <si>
+    <t>ParabolicFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>NiLatticeXvLatticeBm</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting lattice stage. Scan xvlattice. With band mapping.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>BMPDloopTof8000</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>hw_XvLattice</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
     <t>LinearFit1D</t>
   </si>
   <si>
     <t>StdErr</t>
   </si>
   <si>
-    <t>NiLaticeTofCameraOdt</t>
-  </si>
-  <si>
-    <t>A TOF experiment at the non-interacting lattice stage.</t>
-  </si>
-  <si>
-    <t>ODT</t>
-  </si>
-  <si>
-    <t>SideOdtCamera</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>TOF</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>NiLaticeTofCameraOdt</t>
-  </si>
-  <si>
-    <t>A TOF experiment at the non-interacting lattice stage.</t>
-  </si>
-  <si>
-    <t>ODT</t>
-  </si>
-  <si>
-    <t>SideOdtCamera</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>TOF</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>TwoLevelWeakLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>NiLaticeTofCameraOdt</t>
-  </si>
-  <si>
-    <t>A TOF experiment at the non-interacting lattice stage.</t>
-  </si>
-  <si>
-    <t>ODT</t>
-  </si>
-  <si>
-    <t>SideOdtCamera</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>TOF</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>TwoLevelWeakLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>NiBecSlosh</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting BEC stage. Snapping both ODT and XODT off then on.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>Bec</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>NiSloshTime</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>ParabolicFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>NiLatticeXvLatticeBm</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting lattice stage. Scan xvlattice. With band mapping.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>BMPDloopTof8000</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>hw_XvLattice</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
+    <t>ImagingMethod</t>
+  </si>
+  <si>
+    <t>Absorption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3211,7 +3061,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -3219,17 +3069,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3507,34 +3355,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.375" customWidth="true"/>
-    <col min="2" max="2" width="87" customWidth="true"/>
-    <col min="3" max="3" width="14.75" customWidth="true"/>
-    <col min="4" max="4" width="23.75" customWidth="true"/>
-    <col min="5" max="5" width="19.875" customWidth="true"/>
-    <col min="6" max="6" width="8" customWidth="true"/>
-    <col min="7" max="7" width="18.5" customWidth="true"/>
-    <col min="8" max="8" width="31.625" customWidth="true"/>
-    <col min="9" max="9" width="19.375" customWidth="true"/>
-    <col min="10" max="10" width="12.25" customWidth="true"/>
-    <col min="11" max="11" width="17.625" customWidth="true"/>
-    <col min="12" max="12" width="7.625" customWidth="true"/>
-    <col min="13" max="13" width="19.875" customWidth="true"/>
-    <col min="14" max="14" width="16" customWidth="true"/>
-    <col min="15" max="15" width="14.5" customWidth="true"/>
-    <col min="16" max="16" width="15" customWidth="true"/>
-    <col min="17" max="17" width="15.75" customWidth="true"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3566,28 +3415,31 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
+        <v>998</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>708</v>
       </c>
-      <c r="Q1" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.4">
+      <c r="R1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3613,28 +3465,31 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
+        <v>999</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>709</v>
       </c>
-      <c r="Q2" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.4">
+      <c r="R2" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -3663,25 +3518,28 @@
         <v>182</v>
       </c>
       <c r="K3" t="s">
+        <v>999</v>
+      </c>
+      <c r="L3" t="s">
         <v>183</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>184</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>40</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>185</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -3710,25 +3568,28 @@
         <v>238</v>
       </c>
       <c r="K4" t="s">
+        <v>999</v>
+      </c>
+      <c r="L4" t="s">
         <v>239</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>240</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>30</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>241</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3754,25 +3615,28 @@
         <v>30</v>
       </c>
       <c r="K5" t="s">
+        <v>999</v>
+      </c>
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>8</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>30</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>33</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -3798,25 +3662,28 @@
         <v>40</v>
       </c>
       <c r="K6" t="s">
+        <v>999</v>
+      </c>
+      <c r="L6" t="s">
         <v>41</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>8</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>42</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>30</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>43</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -3845,25 +3712,28 @@
         <v>84</v>
       </c>
       <c r="K7" t="s">
+        <v>999</v>
+      </c>
+      <c r="L7" t="s">
         <v>85</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>8</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>86</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>15</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>87</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>624</v>
       </c>
@@ -3895,25 +3765,28 @@
         <v>632</v>
       </c>
       <c r="K8" t="s">
+        <v>999</v>
+      </c>
+      <c r="L8" t="s">
         <v>633</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>8</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>634</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>2</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>635</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -3942,25 +3815,28 @@
         <v>95</v>
       </c>
       <c r="K9" t="s">
+        <v>999</v>
+      </c>
+      <c r="L9" t="s">
         <v>96</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>8</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>97</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>2</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>98</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>445</v>
       </c>
@@ -3992,75 +3868,81 @@
         <v>453</v>
       </c>
       <c r="K10" t="s">
+        <v>999</v>
+      </c>
+      <c r="L10" t="s">
         <v>454</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>8</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>455</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>15</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>456</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>945</v>
+        <v>932</v>
       </c>
       <c r="B11" t="s">
-        <v>946</v>
+        <v>933</v>
       </c>
       <c r="C11" t="s">
-        <v>947</v>
+        <v>934</v>
       </c>
       <c r="D11" t="s">
-        <v>948</v>
+        <v>935</v>
       </c>
       <c r="E11" t="s">
-        <v>949</v>
+        <v>936</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>950</v>
+        <v>937</v>
       </c>
       <c r="H11" t="s">
-        <v>951</v>
+        <v>938</v>
       </c>
       <c r="I11" t="s">
-        <v>952</v>
+        <v>939</v>
       </c>
       <c r="J11" t="s">
-        <v>953</v>
+        <v>940</v>
       </c>
       <c r="K11" t="s">
-        <v>954</v>
-      </c>
-      <c r="L11">
+        <v>999</v>
+      </c>
+      <c r="L11" t="s">
+        <v>941</v>
+      </c>
+      <c r="M11">
         <v>8</v>
       </c>
-      <c r="M11" t="s">
-        <v>955</v>
-      </c>
-      <c r="N11">
+      <c r="N11" t="s">
+        <v>942</v>
+      </c>
+      <c r="O11">
         <v>30</v>
       </c>
-      <c r="O11" t="s">
-        <v>956</v>
-      </c>
       <c r="P11" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="12" x14ac:dyDescent="0.4">
+        <v>943</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>636</v>
       </c>
@@ -4092,25 +3974,28 @@
         <v>644</v>
       </c>
       <c r="K12" t="s">
+        <v>999</v>
+      </c>
+      <c r="L12" t="s">
         <v>645</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>8</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>646</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>30</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>647</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -4139,25 +4024,28 @@
         <v>73</v>
       </c>
       <c r="K13" t="s">
+        <v>999</v>
+      </c>
+      <c r="L13" t="s">
         <v>74</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>8</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>75</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>15</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>76</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -4186,25 +4074,28 @@
         <v>51</v>
       </c>
       <c r="K14" t="s">
+        <v>999</v>
+      </c>
+      <c r="L14" t="s">
         <v>52</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>8</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>53</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>30</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>54</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -4233,25 +4124,28 @@
         <v>62</v>
       </c>
       <c r="K15" t="s">
+        <v>999</v>
+      </c>
+      <c r="L15" t="s">
         <v>63</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>8</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>64</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>15</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>65</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>736</v>
       </c>
@@ -4283,25 +4177,28 @@
         <v>744</v>
       </c>
       <c r="K16" t="s">
+        <v>999</v>
+      </c>
+      <c r="L16" t="s">
         <v>745</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>8</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>746</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>2</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>747</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -4327,25 +4224,28 @@
         <v>106</v>
       </c>
       <c r="K17" t="s">
+        <v>999</v>
+      </c>
+      <c r="L17" t="s">
         <v>107</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>8</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>108</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>30</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>99</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -4374,25 +4274,28 @@
         <v>138</v>
       </c>
       <c r="K18" t="s">
+        <v>999</v>
+      </c>
+      <c r="L18" t="s">
         <v>139</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>8</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>140</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>30</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>141</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="19" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -4421,25 +4324,28 @@
         <v>127</v>
       </c>
       <c r="K19" t="s">
+        <v>999</v>
+      </c>
+      <c r="L19" t="s">
         <v>128</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>8</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>129</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>1</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>130</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -4468,25 +4374,28 @@
         <v>116</v>
       </c>
       <c r="K20" t="s">
+        <v>999</v>
+      </c>
+      <c r="L20" t="s">
         <v>117</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>8</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>118</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>1</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>119</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>749</v>
       </c>
@@ -4518,25 +4427,28 @@
         <v>757</v>
       </c>
       <c r="K21" t="s">
+        <v>999</v>
+      </c>
+      <c r="L21" t="s">
         <v>758</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>8</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>759</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>0.2</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>760</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="22" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -4565,25 +4477,28 @@
         <v>160</v>
       </c>
       <c r="K22" t="s">
+        <v>999</v>
+      </c>
+      <c r="L22" t="s">
         <v>161</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>8</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>162</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>0.2</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>163</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="23" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -4612,25 +4527,28 @@
         <v>171</v>
       </c>
       <c r="K23" t="s">
+        <v>999</v>
+      </c>
+      <c r="L23" t="s">
         <v>172</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>8</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>173</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>0.2</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>174</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="24" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>840</v>
       </c>
@@ -4662,25 +4580,28 @@
         <v>848</v>
       </c>
       <c r="K24" t="s">
+        <v>999</v>
+      </c>
+      <c r="L24" t="s">
         <v>849</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>8</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>850</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>0.5</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>851</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -4709,25 +4630,28 @@
         <v>149</v>
       </c>
       <c r="K25" t="s">
+        <v>999</v>
+      </c>
+      <c r="L25" t="s">
         <v>150</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>8</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>151</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.2</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>152</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="26" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>866</v>
       </c>
@@ -4759,25 +4683,28 @@
         <v>874</v>
       </c>
       <c r="K26" t="s">
+        <v>999</v>
+      </c>
+      <c r="L26" t="s">
         <v>875</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>876</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0.2</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>877</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="27" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>696</v>
       </c>
@@ -4809,25 +4736,28 @@
         <v>704</v>
       </c>
       <c r="K27" t="s">
+        <v>999</v>
+      </c>
+      <c r="L27" t="s">
         <v>705</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>8</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>706</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>200</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>707</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="28" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>266</v>
       </c>
@@ -4859,25 +4789,28 @@
         <v>274</v>
       </c>
       <c r="K28" t="s">
+        <v>999</v>
+      </c>
+      <c r="L28" t="s">
         <v>275</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>8</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>276</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>30</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>277</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="29" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>254</v>
       </c>
@@ -4909,25 +4842,28 @@
         <v>262</v>
       </c>
       <c r="K29" t="s">
+        <v>999</v>
+      </c>
+      <c r="L29" t="s">
         <v>263</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>8</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>264</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>30</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>265</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="30" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>421</v>
       </c>
@@ -4959,25 +4895,28 @@
         <v>429</v>
       </c>
       <c r="K30" t="s">
+        <v>999</v>
+      </c>
+      <c r="L30" t="s">
         <v>430</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>20</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>431</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>0.2</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>432</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="31" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>853</v>
       </c>
@@ -5009,25 +4948,28 @@
         <v>861</v>
       </c>
       <c r="K31" t="s">
+        <v>999</v>
+      </c>
+      <c r="L31" t="s">
         <v>862</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>8</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>863</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>0.2</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>864</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="32" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>529</v>
       </c>
@@ -5059,25 +5001,28 @@
         <v>537</v>
       </c>
       <c r="K32" t="s">
+        <v>999</v>
+      </c>
+      <c r="L32" t="s">
         <v>538</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>2</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>539</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>0.2</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>540</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="33" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>186</v>
       </c>
@@ -5106,25 +5051,28 @@
         <v>193</v>
       </c>
       <c r="K33" t="s">
+        <v>999</v>
+      </c>
+      <c r="L33" t="s">
         <v>194</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>8</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>195</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>0.2</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>196</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="34" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>314</v>
       </c>
@@ -5156,25 +5104,28 @@
         <v>322</v>
       </c>
       <c r="K34" t="s">
+        <v>999</v>
+      </c>
+      <c r="L34" t="s">
         <v>323</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>8</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>324</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>0.2</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>325</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="35" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>198</v>
       </c>
@@ -5203,25 +5154,28 @@
         <v>205</v>
       </c>
       <c r="K35" t="s">
+        <v>999</v>
+      </c>
+      <c r="L35" t="s">
         <v>206</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>8</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>207</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>30</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>208</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="36" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>209</v>
       </c>
@@ -5250,25 +5204,28 @@
         <v>216</v>
       </c>
       <c r="K36" t="s">
+        <v>999</v>
+      </c>
+      <c r="L36" t="s">
         <v>217</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>8</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>218</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>30</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>219</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="37" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>220</v>
       </c>
@@ -5297,25 +5254,28 @@
         <v>227</v>
       </c>
       <c r="K37" t="s">
+        <v>999</v>
+      </c>
+      <c r="L37" t="s">
         <v>228</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>12</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>229</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>0.2</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>230</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="38" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -5347,25 +5307,28 @@
         <v>250</v>
       </c>
       <c r="K38" t="s">
+        <v>999</v>
+      </c>
+      <c r="L38" t="s">
         <v>251</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>8</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>252</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>30</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>253</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="39" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>648</v>
       </c>
@@ -5397,25 +5360,28 @@
         <v>656</v>
       </c>
       <c r="K39" t="s">
+        <v>999</v>
+      </c>
+      <c r="L39" t="s">
         <v>657</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>8</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>658</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>30</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>659</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="40" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>576</v>
       </c>
@@ -5447,25 +5413,28 @@
         <v>584</v>
       </c>
       <c r="K40" t="s">
+        <v>999</v>
+      </c>
+      <c r="L40" t="s">
         <v>585</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>8</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>586</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>0.2</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>587</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="41" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>326</v>
       </c>
@@ -5497,25 +5466,28 @@
         <v>334</v>
       </c>
       <c r="K41" t="s">
+        <v>999</v>
+      </c>
+      <c r="L41" t="s">
         <v>335</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>8</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>336</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>30</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>337</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="42" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>433</v>
       </c>
@@ -5547,25 +5519,28 @@
         <v>441</v>
       </c>
       <c r="K42" t="s">
+        <v>999</v>
+      </c>
+      <c r="L42" t="s">
         <v>442</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>8</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>443</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>1</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>444</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="43" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>879</v>
       </c>
@@ -5597,76 +5572,81 @@
         <v>887</v>
       </c>
       <c r="K43" t="s">
+        <v>999</v>
+      </c>
+      <c r="L43" t="s">
         <v>888</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>2</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>889</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>0.2</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>890</v>
       </c>
-      <c r="P43" t="s">
+      <c r="Q43" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="44" x14ac:dyDescent="0.4">
-      <c r="A44" s="0" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>1038</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>1041</v>
-      </c>
-      <c r="F44" s="0">
-        <v>4</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>1042</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>1043</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>1044</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>1045</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>1046</v>
-      </c>
-      <c r="L44" s="0">
-        <v>4</v>
-      </c>
-      <c r="M44" s="0" t="s">
-        <v>1047</v>
-      </c>
-      <c r="N44" s="0">
+    <row r="44" spans="1:17">
+      <c r="A44" t="s">
+        <v>985</v>
+      </c>
+      <c r="B44" t="s">
+        <v>986</v>
+      </c>
+      <c r="C44" t="s">
+        <v>987</v>
+      </c>
+      <c r="D44" t="s">
+        <v>988</v>
+      </c>
+      <c r="E44" t="s">
+        <v>989</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>990</v>
+      </c>
+      <c r="H44" t="s">
+        <v>991</v>
+      </c>
+      <c r="I44" t="s">
+        <v>992</v>
+      </c>
+      <c r="J44" t="s">
+        <v>993</v>
+      </c>
+      <c r="K44" t="s">
+        <v>999</v>
+      </c>
+      <c r="L44" t="s">
+        <v>994</v>
+      </c>
+      <c r="M44">
+        <v>4</v>
+      </c>
+      <c r="N44" t="s">
+        <v>995</v>
+      </c>
+      <c r="O44">
         <v>1</v>
       </c>
-      <c r="O44" s="0" t="s">
-        <v>1048</v>
-      </c>
-      <c r="P44" s="0" t="s">
-        <v>1049</v>
-      </c>
-      <c r="Q44" s="0"/>
-    </row>
-    <row r="45" x14ac:dyDescent="0.4">
+      <c r="P44" t="s">
+        <v>996</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>278</v>
       </c>
@@ -5698,25 +5678,28 @@
         <v>286</v>
       </c>
       <c r="K45" t="s">
+        <v>999</v>
+      </c>
+      <c r="L45" t="s">
         <v>287</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>8</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>288</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>0.2</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>289</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="46" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>290</v>
       </c>
@@ -5748,25 +5731,28 @@
         <v>298</v>
       </c>
       <c r="K46" t="s">
+        <v>999</v>
+      </c>
+      <c r="L46" t="s">
         <v>299</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>8</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>300</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>10</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>301</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="47" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>302</v>
       </c>
@@ -5798,25 +5784,28 @@
         <v>310</v>
       </c>
       <c r="K47" t="s">
+        <v>999</v>
+      </c>
+      <c r="L47" t="s">
         <v>311</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>12</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
         <v>312</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>1</v>
       </c>
-      <c r="O47" t="s">
+      <c r="P47" t="s">
         <v>313</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="48" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>588</v>
       </c>
@@ -5848,25 +5837,28 @@
         <v>596</v>
       </c>
       <c r="K48" t="s">
+        <v>999</v>
+      </c>
+      <c r="L48" t="s">
         <v>597</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>0.5</v>
       </c>
-      <c r="M48" t="s">
+      <c r="N48" t="s">
         <v>598</v>
       </c>
-      <c r="N48">
+      <c r="O48">
         <v>0.2</v>
       </c>
-      <c r="O48" t="s">
+      <c r="P48" t="s">
         <v>599</v>
       </c>
-      <c r="P48" t="s">
+      <c r="Q48" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="49" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>338</v>
       </c>
@@ -5898,25 +5890,28 @@
         <v>346</v>
       </c>
       <c r="K49" t="s">
+        <v>999</v>
+      </c>
+      <c r="L49" t="s">
         <v>347</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>8</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49" t="s">
         <v>348</v>
       </c>
-      <c r="N49">
+      <c r="O49">
         <v>30</v>
       </c>
-      <c r="O49" t="s">
+      <c r="P49" t="s">
         <v>349</v>
       </c>
-      <c r="P49" t="s">
+      <c r="Q49" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="50" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>350</v>
       </c>
@@ -5948,25 +5943,28 @@
         <v>358</v>
       </c>
       <c r="K50" t="s">
+        <v>999</v>
+      </c>
+      <c r="L50" t="s">
         <v>359</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>8</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>360</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>1</v>
       </c>
-      <c r="O50" t="s">
+      <c r="P50" t="s">
         <v>361</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="51" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>362</v>
       </c>
@@ -5998,25 +5996,28 @@
         <v>370</v>
       </c>
       <c r="K51" t="s">
+        <v>999</v>
+      </c>
+      <c r="L51" t="s">
         <v>371</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>8</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" t="s">
         <v>372</v>
       </c>
-      <c r="N51">
+      <c r="O51">
         <v>0.2</v>
       </c>
-      <c r="O51" t="s">
+      <c r="P51" t="s">
         <v>373</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="52" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>374</v>
       </c>
@@ -6048,25 +6049,28 @@
         <v>382</v>
       </c>
       <c r="K52" t="s">
+        <v>999</v>
+      </c>
+      <c r="L52" t="s">
         <v>383</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>8</v>
       </c>
-      <c r="M52" t="s">
+      <c r="N52" t="s">
         <v>384</v>
       </c>
-      <c r="N52">
+      <c r="O52">
         <v>0.2</v>
       </c>
-      <c r="O52" t="s">
+      <c r="P52" t="s">
         <v>385</v>
       </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="53" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>386</v>
       </c>
@@ -6095,25 +6099,28 @@
         <v>393</v>
       </c>
       <c r="K53" t="s">
+        <v>999</v>
+      </c>
+      <c r="L53" t="s">
         <v>394</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>8</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>395</v>
       </c>
-      <c r="N53">
+      <c r="O53">
         <v>30</v>
       </c>
-      <c r="O53" t="s">
+      <c r="P53" t="s">
         <v>396</v>
       </c>
-      <c r="P53" t="s">
+      <c r="Q53" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="54" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>397</v>
       </c>
@@ -6145,25 +6152,28 @@
         <v>405</v>
       </c>
       <c r="K54" t="s">
+        <v>999</v>
+      </c>
+      <c r="L54" t="s">
         <v>406</v>
       </c>
-      <c r="L54">
+      <c r="M54">
         <v>8</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>407</v>
       </c>
-      <c r="N54">
+      <c r="O54">
         <v>0.2</v>
       </c>
-      <c r="O54" t="s">
+      <c r="P54" t="s">
         <v>408</v>
       </c>
-      <c r="P54" t="s">
+      <c r="Q54" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="55" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -6195,25 +6205,28 @@
         <v>417</v>
       </c>
       <c r="K55" t="s">
+        <v>999</v>
+      </c>
+      <c r="L55" t="s">
         <v>418</v>
       </c>
-      <c r="L55">
+      <c r="M55">
         <v>8</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>419</v>
       </c>
-      <c r="N55">
+      <c r="O55">
         <v>0.2</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>420</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="56" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>600</v>
       </c>
@@ -6245,25 +6258,28 @@
         <v>608</v>
       </c>
       <c r="K56" t="s">
+        <v>999</v>
+      </c>
+      <c r="L56" t="s">
         <v>609</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>1</v>
       </c>
-      <c r="M56" t="s">
+      <c r="N56" t="s">
         <v>610</v>
       </c>
-      <c r="N56">
+      <c r="O56">
         <v>0.2</v>
       </c>
-      <c r="O56" t="s">
+      <c r="P56" t="s">
         <v>611</v>
       </c>
-      <c r="P56" t="s">
+      <c r="Q56" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="57" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>457</v>
       </c>
@@ -6295,25 +6311,28 @@
         <v>465</v>
       </c>
       <c r="K57" t="s">
+        <v>999</v>
+      </c>
+      <c r="L57" t="s">
         <v>466</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>8</v>
       </c>
-      <c r="M57" t="s">
+      <c r="N57" t="s">
         <v>467</v>
       </c>
-      <c r="N57">
+      <c r="O57">
         <v>0.2</v>
       </c>
-      <c r="O57" t="s">
+      <c r="P57" t="s">
         <v>468</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="58" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>469</v>
       </c>
@@ -6345,25 +6364,28 @@
         <v>477</v>
       </c>
       <c r="K58" t="s">
+        <v>999</v>
+      </c>
+      <c r="L58" t="s">
         <v>478</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>8</v>
       </c>
-      <c r="M58" t="s">
+      <c r="N58" t="s">
         <v>479</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>2</v>
       </c>
-      <c r="O58" t="s">
+      <c r="P58" t="s">
         <v>480</v>
       </c>
-      <c r="P58" t="s">
+      <c r="Q58" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="59" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>481</v>
       </c>
@@ -6395,25 +6417,28 @@
         <v>489</v>
       </c>
       <c r="K59" t="s">
+        <v>999</v>
+      </c>
+      <c r="L59" t="s">
         <v>490</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>8</v>
       </c>
-      <c r="M59" t="s">
+      <c r="N59" t="s">
         <v>491</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>2</v>
       </c>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
         <v>492</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="60" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>493</v>
       </c>
@@ -6445,25 +6470,28 @@
         <v>501</v>
       </c>
       <c r="K60" t="s">
+        <v>999</v>
+      </c>
+      <c r="L60" t="s">
         <v>502</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>8</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>503</v>
       </c>
-      <c r="N60">
+      <c r="O60">
         <v>30</v>
       </c>
-      <c r="O60" t="s">
+      <c r="P60" t="s">
         <v>504</v>
       </c>
-      <c r="P60" t="s">
+      <c r="Q60" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="61" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>505</v>
       </c>
@@ -6495,25 +6523,28 @@
         <v>513</v>
       </c>
       <c r="K61" t="s">
+        <v>999</v>
+      </c>
+      <c r="L61" t="s">
         <v>514</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>8</v>
       </c>
-      <c r="M61" t="s">
+      <c r="N61" t="s">
         <v>515</v>
       </c>
-      <c r="N61">
+      <c r="O61">
         <v>2</v>
       </c>
-      <c r="O61" t="s">
+      <c r="P61" t="s">
         <v>516</v>
       </c>
-      <c r="P61" t="s">
+      <c r="Q61" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="62" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>517</v>
       </c>
@@ -6545,25 +6576,28 @@
         <v>525</v>
       </c>
       <c r="K62" t="s">
+        <v>999</v>
+      </c>
+      <c r="L62" t="s">
         <v>526</v>
       </c>
-      <c r="L62">
+      <c r="M62">
         <v>8</v>
       </c>
-      <c r="M62" t="s">
+      <c r="N62" t="s">
         <v>527</v>
       </c>
-      <c r="N62">
+      <c r="O62">
         <v>15</v>
       </c>
-      <c r="O62" t="s">
+      <c r="P62" t="s">
         <v>528</v>
       </c>
-      <c r="P62" t="s">
+      <c r="Q62" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="63" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>541</v>
       </c>
@@ -6592,25 +6626,28 @@
         <v>548</v>
       </c>
       <c r="K63" t="s">
+        <v>999</v>
+      </c>
+      <c r="L63" t="s">
         <v>549</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>8</v>
       </c>
-      <c r="M63" t="s">
+      <c r="N63" t="s">
         <v>550</v>
       </c>
-      <c r="N63">
+      <c r="O63">
         <v>30</v>
       </c>
-      <c r="O63" t="s">
+      <c r="P63" t="s">
         <v>551</v>
       </c>
-      <c r="P63" t="s">
+      <c r="Q63" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="64" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>552</v>
       </c>
@@ -6642,25 +6679,28 @@
         <v>560</v>
       </c>
       <c r="K64" t="s">
+        <v>999</v>
+      </c>
+      <c r="L64" t="s">
         <v>561</v>
       </c>
-      <c r="L64">
+      <c r="M64">
         <v>8</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>562</v>
       </c>
-      <c r="N64">
+      <c r="O64">
         <v>30</v>
       </c>
-      <c r="O64" t="s">
+      <c r="P64" t="s">
         <v>563</v>
       </c>
-      <c r="P64" t="s">
+      <c r="Q64" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="65" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>564</v>
       </c>
@@ -6692,25 +6732,28 @@
         <v>572</v>
       </c>
       <c r="K65" t="s">
+        <v>999</v>
+      </c>
+      <c r="L65" t="s">
         <v>573</v>
       </c>
-      <c r="L65">
+      <c r="M65">
         <v>8</v>
       </c>
-      <c r="M65" t="s">
+      <c r="N65" t="s">
         <v>574</v>
       </c>
-      <c r="N65">
+      <c r="O65">
         <v>2</v>
       </c>
-      <c r="O65" t="s">
+      <c r="P65" t="s">
         <v>575</v>
       </c>
-      <c r="P65" t="s">
+      <c r="Q65" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="66" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>918</v>
       </c>
@@ -6742,25 +6785,28 @@
         <v>926</v>
       </c>
       <c r="K66" t="s">
+        <v>999</v>
+      </c>
+      <c r="L66" t="s">
         <v>927</v>
       </c>
-      <c r="L66">
+      <c r="M66">
         <v>8</v>
       </c>
-      <c r="M66" t="s">
+      <c r="N66" t="s">
         <v>928</v>
       </c>
-      <c r="N66">
+      <c r="O66">
         <v>1</v>
       </c>
-      <c r="O66" t="s">
+      <c r="P66" t="s">
         <v>929</v>
       </c>
-      <c r="P66" t="s">
+      <c r="Q66" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="67" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>612</v>
       </c>
@@ -6792,25 +6838,28 @@
         <v>620</v>
       </c>
       <c r="K67" t="s">
+        <v>999</v>
+      </c>
+      <c r="L67" t="s">
         <v>621</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>8</v>
       </c>
-      <c r="M67" t="s">
+      <c r="N67" t="s">
         <v>622</v>
       </c>
-      <c r="N67">
+      <c r="O67">
         <v>1</v>
       </c>
-      <c r="O67" t="s">
+      <c r="P67" t="s">
         <v>623</v>
       </c>
-      <c r="P67" t="s">
+      <c r="Q67" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="68" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>775</v>
       </c>
@@ -6842,25 +6891,28 @@
         <v>783</v>
       </c>
       <c r="K68" t="s">
+        <v>999</v>
+      </c>
+      <c r="L68" t="s">
         <v>784</v>
       </c>
-      <c r="L68">
+      <c r="M68">
         <v>2</v>
       </c>
-      <c r="M68" t="s">
+      <c r="N68" t="s">
         <v>785</v>
       </c>
-      <c r="N68">
+      <c r="O68">
         <v>0.2</v>
       </c>
-      <c r="O68" t="s">
+      <c r="P68" t="s">
         <v>786</v>
       </c>
-      <c r="P68" t="s">
+      <c r="Q68" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="69" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>905</v>
       </c>
@@ -6892,25 +6944,28 @@
         <v>913</v>
       </c>
       <c r="K69" t="s">
+        <v>999</v>
+      </c>
+      <c r="L69" t="s">
         <v>914</v>
       </c>
-      <c r="L69">
+      <c r="M69">
         <v>8</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>915</v>
       </c>
-      <c r="N69">
+      <c r="O69">
         <v>15</v>
       </c>
-      <c r="O69" t="s">
+      <c r="P69" t="s">
         <v>916</v>
       </c>
-      <c r="P69" t="s">
+      <c r="Q69" t="s">
         <v>917</v>
       </c>
     </row>
-    <row r="70" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>672</v>
       </c>
@@ -6942,25 +6997,28 @@
         <v>680</v>
       </c>
       <c r="K70" t="s">
+        <v>999</v>
+      </c>
+      <c r="L70" t="s">
         <v>681</v>
       </c>
-      <c r="L70">
+      <c r="M70">
         <v>8</v>
       </c>
-      <c r="M70" t="s">
+      <c r="N70" t="s">
         <v>682</v>
       </c>
-      <c r="N70">
+      <c r="O70">
         <v>15</v>
       </c>
-      <c r="O70" t="s">
+      <c r="P70" t="s">
         <v>683</v>
       </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="71" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>660</v>
       </c>
@@ -6992,25 +7050,28 @@
         <v>668</v>
       </c>
       <c r="K71" t="s">
+        <v>999</v>
+      </c>
+      <c r="L71" t="s">
         <v>669</v>
       </c>
-      <c r="L71">
+      <c r="M71">
         <v>8</v>
       </c>
-      <c r="M71" t="s">
+      <c r="N71" t="s">
         <v>670</v>
       </c>
-      <c r="N71">
+      <c r="O71">
         <v>30</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>671</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="72" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>684</v>
       </c>
@@ -7042,25 +7103,28 @@
         <v>692</v>
       </c>
       <c r="K72" t="s">
+        <v>999</v>
+      </c>
+      <c r="L72" t="s">
         <v>693</v>
       </c>
-      <c r="L72">
+      <c r="M72">
         <v>8</v>
       </c>
-      <c r="M72" t="s">
+      <c r="N72" t="s">
         <v>694</v>
       </c>
-      <c r="N72">
+      <c r="O72">
         <v>30</v>
       </c>
-      <c r="O72" t="s">
+      <c r="P72" t="s">
         <v>695</v>
       </c>
-      <c r="P72" t="s">
+      <c r="Q72" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="73" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>710</v>
       </c>
@@ -7092,25 +7156,28 @@
         <v>718</v>
       </c>
       <c r="K73" t="s">
+        <v>999</v>
+      </c>
+      <c r="L73" t="s">
         <v>719</v>
       </c>
-      <c r="L73">
+      <c r="M73">
         <v>8</v>
       </c>
-      <c r="M73" t="s">
+      <c r="N73" t="s">
         <v>720</v>
       </c>
-      <c r="N73">
+      <c r="O73">
         <v>0.2</v>
       </c>
-      <c r="O73" t="s">
+      <c r="P73" t="s">
         <v>721</v>
       </c>
-      <c r="P73" t="s">
+      <c r="Q73" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="74" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>723</v>
       </c>
@@ -7142,25 +7209,28 @@
         <v>731</v>
       </c>
       <c r="K74" t="s">
+        <v>999</v>
+      </c>
+      <c r="L74" t="s">
         <v>732</v>
       </c>
-      <c r="L74">
+      <c r="M74">
         <v>8</v>
       </c>
-      <c r="M74" t="s">
+      <c r="N74" t="s">
         <v>733</v>
       </c>
-      <c r="N74">
+      <c r="O74">
         <v>2</v>
       </c>
-      <c r="O74" t="s">
+      <c r="P74" t="s">
         <v>734</v>
       </c>
-      <c r="P74" t="s">
+      <c r="Q74" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="75" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>762</v>
       </c>
@@ -7192,25 +7262,28 @@
         <v>770</v>
       </c>
       <c r="K75" t="s">
+        <v>999</v>
+      </c>
+      <c r="L75" t="s">
         <v>771</v>
       </c>
-      <c r="L75">
+      <c r="M75">
         <v>2</v>
       </c>
-      <c r="M75" t="s">
+      <c r="N75" t="s">
         <v>772</v>
       </c>
-      <c r="N75">
+      <c r="O75">
         <v>0.2</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>773</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="76" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>788</v>
       </c>
@@ -7242,25 +7315,28 @@
         <v>796</v>
       </c>
       <c r="K76" t="s">
+        <v>999</v>
+      </c>
+      <c r="L76" t="s">
         <v>797</v>
       </c>
-      <c r="L76">
+      <c r="M76">
         <v>8</v>
       </c>
-      <c r="M76" t="s">
+      <c r="N76" t="s">
         <v>798</v>
       </c>
-      <c r="N76">
+      <c r="O76">
         <v>0.2</v>
       </c>
-      <c r="O76" t="s">
+      <c r="P76" t="s">
         <v>799</v>
       </c>
-      <c r="P76" t="s">
+      <c r="Q76" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="77" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>801</v>
       </c>
@@ -7292,25 +7368,28 @@
         <v>809</v>
       </c>
       <c r="K77" t="s">
+        <v>999</v>
+      </c>
+      <c r="L77" t="s">
         <v>810</v>
       </c>
-      <c r="L77">
+      <c r="M77">
         <v>2</v>
       </c>
-      <c r="M77" t="s">
+      <c r="N77" t="s">
         <v>811</v>
       </c>
-      <c r="N77">
+      <c r="O77">
         <v>0.2</v>
       </c>
-      <c r="O77" t="s">
+      <c r="P77" t="s">
         <v>812</v>
       </c>
-      <c r="P77" t="s">
+      <c r="Q77" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="78" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>814</v>
       </c>
@@ -7342,25 +7421,28 @@
         <v>822</v>
       </c>
       <c r="K78" t="s">
+        <v>999</v>
+      </c>
+      <c r="L78" t="s">
         <v>823</v>
       </c>
-      <c r="L78">
+      <c r="M78">
         <v>8</v>
       </c>
-      <c r="M78" t="s">
+      <c r="N78" t="s">
         <v>824</v>
       </c>
-      <c r="N78">
+      <c r="O78">
         <v>15</v>
       </c>
-      <c r="O78" t="s">
+      <c r="P78" t="s">
         <v>825</v>
       </c>
-      <c r="P78" t="s">
+      <c r="Q78" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="79" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>827</v>
       </c>
@@ -7392,25 +7474,28 @@
         <v>835</v>
       </c>
       <c r="K79" t="s">
+        <v>999</v>
+      </c>
+      <c r="L79" t="s">
         <v>836</v>
       </c>
-      <c r="L79">
+      <c r="M79">
         <v>8</v>
       </c>
-      <c r="M79" t="s">
+      <c r="N79" t="s">
         <v>837</v>
       </c>
-      <c r="N79">
+      <c r="O79">
         <v>2</v>
       </c>
-      <c r="O79" t="s">
+      <c r="P79" t="s">
         <v>838</v>
       </c>
-      <c r="P79" t="s">
+      <c r="Q79" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="80" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:17">
       <c r="A80" t="s">
         <v>892</v>
       </c>
@@ -7442,176 +7527,185 @@
         <v>900</v>
       </c>
       <c r="K80" t="s">
+        <v>999</v>
+      </c>
+      <c r="L80" t="s">
         <v>901</v>
       </c>
-      <c r="L80">
+      <c r="M80">
         <v>2</v>
       </c>
-      <c r="M80" t="s">
+      <c r="N80" t="s">
         <v>902</v>
       </c>
-      <c r="N80">
+      <c r="O80">
         <v>0.2</v>
       </c>
-      <c r="O80" t="s">
+      <c r="P80" t="s">
         <v>903</v>
       </c>
-      <c r="P80" t="s">
+      <c r="Q80" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:17">
+      <c r="A81" t="s">
+        <v>946</v>
+      </c>
+      <c r="B81" t="s">
+        <v>947</v>
+      </c>
+      <c r="C81" t="s">
+        <v>948</v>
+      </c>
+      <c r="D81" t="s">
+        <v>949</v>
+      </c>
+      <c r="E81" t="s">
+        <v>950</v>
+      </c>
+      <c r="F81">
+        <v>4</v>
+      </c>
+      <c r="G81" t="s">
+        <v>951</v>
+      </c>
+      <c r="H81" t="s">
+        <v>952</v>
+      </c>
+      <c r="I81" t="s">
+        <v>953</v>
+      </c>
+      <c r="J81" t="s">
+        <v>954</v>
+      </c>
+      <c r="K81" t="s">
+        <v>999</v>
+      </c>
+      <c r="L81" t="s">
+        <v>955</v>
+      </c>
+      <c r="M81">
+        <v>8</v>
+      </c>
+      <c r="N81" t="s">
+        <v>956</v>
+      </c>
+      <c r="O81">
+        <v>0.2</v>
+      </c>
+      <c r="P81" t="s">
+        <v>957</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
+      <c r="A82" t="s">
         <v>959</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B82" t="s">
         <v>960</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C82" t="s">
         <v>961</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D82" t="s">
         <v>962</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E82" t="s">
         <v>963</v>
       </c>
-      <c r="F81" s="0">
-        <v>4</v>
-      </c>
-      <c r="G81" s="0" t="s">
+      <c r="F82">
+        <v>4</v>
+      </c>
+      <c r="G82" t="s">
         <v>964</v>
       </c>
-      <c r="H81" s="0" t="s">
+      <c r="H82" t="s">
         <v>965</v>
       </c>
-      <c r="I81" s="0" t="s">
+      <c r="I82" t="s">
         <v>966</v>
       </c>
-      <c r="J81" s="0" t="s">
+      <c r="J82" t="s">
         <v>967</v>
       </c>
-      <c r="K81" s="0" t="s">
+      <c r="K82" t="s">
+        <v>999</v>
+      </c>
+      <c r="L82" t="s">
         <v>968</v>
       </c>
-      <c r="L81" s="0">
+      <c r="M82">
+        <v>0.5</v>
+      </c>
+      <c r="N82" t="s">
+        <v>969</v>
+      </c>
+      <c r="O82">
+        <v>0.2</v>
+      </c>
+      <c r="P82" t="s">
+        <v>970</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" t="s">
+        <v>972</v>
+      </c>
+      <c r="B83" t="s">
+        <v>973</v>
+      </c>
+      <c r="C83" t="s">
+        <v>974</v>
+      </c>
+      <c r="D83" t="s">
+        <v>975</v>
+      </c>
+      <c r="E83" t="s">
+        <v>976</v>
+      </c>
+      <c r="F83">
+        <v>4</v>
+      </c>
+      <c r="G83" t="s">
+        <v>977</v>
+      </c>
+      <c r="H83" t="s">
+        <v>978</v>
+      </c>
+      <c r="I83" t="s">
+        <v>979</v>
+      </c>
+      <c r="J83" t="s">
+        <v>980</v>
+      </c>
+      <c r="K83" t="s">
+        <v>999</v>
+      </c>
+      <c r="L83" t="s">
+        <v>981</v>
+      </c>
+      <c r="M83">
         <v>8</v>
       </c>
-      <c r="M81" s="0" t="s">
-        <v>969</v>
-      </c>
-      <c r="N81" s="0">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="O81" s="0" t="s">
-        <v>970</v>
-      </c>
-      <c r="P81" s="0" t="s">
-        <v>971</v>
-      </c>
-      <c r="Q81" s="0"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="0" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>1015</v>
-      </c>
-      <c r="F82" s="0">
-        <v>4</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>1016</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>1017</v>
-      </c>
-      <c r="I82" s="0" t="s">
-        <v>1018</v>
-      </c>
-      <c r="J82" s="0" t="s">
-        <v>1019</v>
-      </c>
-      <c r="K82" s="0" t="s">
-        <v>1020</v>
-      </c>
-      <c r="L82" s="0">
-        <v>0.5</v>
-      </c>
-      <c r="M82" s="0" t="s">
-        <v>1021</v>
-      </c>
-      <c r="N82" s="0">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="O82" s="0" t="s">
-        <v>1022</v>
-      </c>
-      <c r="P82" s="0" t="s">
-        <v>1023</v>
-      </c>
-      <c r="Q82" s="0"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="0" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>1026</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>1027</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>1028</v>
-      </c>
-      <c r="F83" s="0">
-        <v>4</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>1029</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>1030</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>1032</v>
-      </c>
-      <c r="K83" s="0" t="s">
-        <v>1033</v>
-      </c>
-      <c r="L83" s="0">
-        <v>8</v>
-      </c>
-      <c r="M83" s="0" t="s">
-        <v>1034</v>
-      </c>
-      <c r="N83" s="0">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="O83" s="0" t="s">
-        <v>1035</v>
-      </c>
-      <c r="P83" s="0" t="s">
-        <v>1036</v>
-      </c>
-      <c r="Q83" s="0"/>
+      <c r="N83" t="s">
+        <v>982</v>
+      </c>
+      <c r="O83">
+        <v>0.2</v>
+      </c>
+      <c r="P83" t="s">
+        <v>983</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>984</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
modified the default setConfig
</commit_message>
<xml_diff>
--- a/config/becExpConfig/becExpType.csv.xlsx
+++ b/config/becExpConfig/becExpType.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoc\Documents\MMUser\config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weld Lab User\Documents\MMUser\config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC5C255-F223-4F65-A6AA-952D6AB280EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCB21F2-CC93-421D-8955-392F383D2C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>TrialName</t>
   </si>
@@ -124,23 +124,29 @@
   <si>
     <t>DensityFit</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImagingMethod</t>
+  </si>
+  <si>
+    <t>Absorption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -171,7 +177,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,34 +455,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.3984375" customWidth="1"/>
-    <col min="2" max="2" width="95.265625" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="95.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" customWidth="1"/>
-    <col min="8" max="8" width="35.1328125" customWidth="1"/>
-    <col min="9" max="9" width="21.3984375" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="7.86328125" customWidth="1"/>
-    <col min="13" max="13" width="20.3984375" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="15" max="15" width="16.3984375" customWidth="1"/>
-    <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="16.86328125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,28 +515,31 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -561,24 +571,27 @@
         <v>18</v>
       </c>
       <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed server IP address
</commit_message>
<xml_diff>
--- a/config/becExpConfig/becExpType.csv.xlsx
+++ b/config/becExpConfig/becExpType.csv.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5050C-A9FC-4E53-9A5E-BB48C24F7D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="1109">
   <si>
     <t>TrialName</t>
   </si>
@@ -3314,6 +3314,51 @@
   </si>
   <si>
     <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingHf</t>
+  </si>
+  <si>
+    <t>EvapD</t>
+  </si>
+  <si>
+    <t>An experiment at evaporation stage D.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>CiceroLogTime</t>
+  </si>
+  <si>
+    <t>AtomNumber;DensityFit;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[549 1745;903 1905;1286 1930;1532 1678;1603 1325;1617 1085;1501 850;1355 743;908 715;693 740;535 925;522 1284]</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
   </si>
 </sst>
 </file>
@@ -3344,7 +3389,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3352,12 +3397,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3640,35 +3687,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="87.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="127.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="82.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="true"/>
+    <col min="2" max="2" width="95.28515625" customWidth="true"/>
+    <col min="3" max="3" width="16.42578125" customWidth="true"/>
+    <col min="4" max="4" width="25.7109375" customWidth="true"/>
+    <col min="5" max="5" width="21.42578125" customWidth="true"/>
+    <col min="6" max="6" width="8" customWidth="true"/>
+    <col min="7" max="7" width="19.5703125" customWidth="true"/>
+    <col min="8" max="8" width="35.140625" customWidth="true"/>
+    <col min="9" max="9" width="21.42578125" customWidth="true"/>
+    <col min="10" max="10" width="130" customWidth="true"/>
+    <col min="11" max="11" width="13" customWidth="true"/>
+    <col min="12" max="12" width="15.140625" customWidth="true"/>
+    <col min="13" max="13" width="19" customWidth="true"/>
+    <col min="14" max="14" width="7.85546875" customWidth="true"/>
+    <col min="15" max="15" width="20.42578125" customWidth="true"/>
+    <col min="16" max="16" width="17.42578125" customWidth="true"/>
+    <col min="17" max="17" width="16.42578125" customWidth="true"/>
+    <col min="18" max="18" width="17" customWidth="true"/>
+    <col min="19" max="19" width="16.85546875" customWidth="true"/>
+    <col min="20" max="20" width="84.28515625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3730,7 +3777,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -3777,7 +3824,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3824,63 +3871,65 @@
         <v>457</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>762</v>
-      </c>
-      <c r="B4" t="s">
-        <v>763</v>
-      </c>
-      <c r="C4" t="s">
-        <v>764</v>
-      </c>
-      <c r="D4" t="s">
-        <v>765</v>
-      </c>
-      <c r="E4" t="s">
-        <v>766</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>767</v>
-      </c>
-      <c r="H4" t="s">
-        <v>768</v>
-      </c>
-      <c r="I4" t="s">
-        <v>769</v>
-      </c>
-      <c r="J4" t="s">
-        <v>770</v>
-      </c>
-      <c r="K4" t="s">
-        <v>771</v>
-      </c>
-      <c r="L4" t="s">
-        <v>772</v>
-      </c>
-      <c r="M4" t="s">
-        <v>773</v>
-      </c>
-      <c r="N4">
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F4" s="0">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N4" s="0">
         <v>8</v>
       </c>
-      <c r="O4" t="s">
-        <v>774</v>
-      </c>
-      <c r="P4">
-        <v>30</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>775</v>
-      </c>
-      <c r="R4" t="s">
-        <v>776</v>
-      </c>
+      <c r="O4" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="P4" s="0">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5">
       <c r="A5" t="s">
         <v>396</v>
       </c>
@@ -3933,7 +3982,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6">
       <c r="A6" t="s">
         <v>289</v>
       </c>
@@ -3986,7 +4035,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -4036,7 +4085,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8">
       <c r="A8" t="s">
         <v>647</v>
       </c>
@@ -4089,7 +4138,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9">
       <c r="A9" t="s">
         <v>408</v>
       </c>
@@ -4142,7 +4191,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -4192,7 +4241,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11">
       <c r="A11" t="s">
         <v>420</v>
       </c>
@@ -4245,7 +4294,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12">
       <c r="A12" t="s">
         <v>122</v>
       </c>
@@ -4298,7 +4347,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13">
       <c r="A13" t="s">
         <v>206</v>
       </c>
@@ -4351,7 +4400,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14">
       <c r="A14" t="s">
         <v>618</v>
       </c>
@@ -4404,7 +4453,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -4454,7 +4503,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4501,7 +4550,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17">
       <c r="A17" t="s">
         <v>1079</v>
       </c>
@@ -4557,7 +4606,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18">
       <c r="A18" t="s">
         <v>301</v>
       </c>
@@ -4613,7 +4662,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19">
       <c r="A19" t="s">
         <v>348</v>
       </c>
@@ -4669,7 +4718,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20">
       <c r="A20" t="s">
         <v>632</v>
       </c>
@@ -4728,7 +4777,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21">
       <c r="A21" t="s">
         <v>911</v>
       </c>
@@ -4787,7 +4836,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22">
       <c r="A22" t="s">
         <v>484</v>
       </c>
@@ -4843,7 +4892,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23">
       <c r="A23" t="s">
         <v>277</v>
       </c>
@@ -4899,7 +4948,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24">
       <c r="A24" t="s">
         <v>471</v>
       </c>
@@ -4955,7 +5004,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25">
       <c r="A25" t="s">
         <v>549</v>
       </c>
@@ -5011,7 +5060,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26">
       <c r="A26" t="s">
         <v>1031</v>
       </c>
@@ -5067,7 +5116,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27">
       <c r="A27" t="s">
         <v>254</v>
       </c>
@@ -5117,7 +5166,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28">
       <c r="A28" t="s">
         <v>337</v>
       </c>
@@ -5167,7 +5216,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -5217,7 +5266,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30">
       <c r="A30" t="s">
         <v>1063</v>
       </c>
@@ -5276,7 +5325,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31">
       <c r="A31" t="s">
         <v>360</v>
       </c>
@@ -5332,7 +5381,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32">
       <c r="A32" t="s">
         <v>851</v>
       </c>
@@ -5391,7 +5440,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33">
       <c r="A33" t="s">
         <v>170</v>
       </c>
@@ -5447,7 +5496,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34">
       <c r="A34" t="s">
         <v>748</v>
       </c>
@@ -5503,7 +5552,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35">
       <c r="A35" t="s">
         <v>821</v>
       </c>
@@ -5562,7 +5611,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -5618,7 +5667,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -5674,7 +5723,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38">
       <c r="A38" t="s">
         <v>836</v>
       </c>
@@ -5733,7 +5782,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39">
       <c r="A39" t="s">
         <v>458</v>
       </c>
@@ -5789,7 +5838,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40">
       <c r="A40" t="s">
         <v>602</v>
       </c>
@@ -5845,7 +5894,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41">
       <c r="A41" t="s">
         <v>661</v>
       </c>
@@ -5901,7 +5950,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42">
       <c r="A42" t="s">
         <v>589</v>
       </c>
@@ -5957,7 +6006,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43">
       <c r="A43" t="s">
         <v>792</v>
       </c>
@@ -6013,7 +6062,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -6069,7 +6118,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45">
       <c r="A45" t="s">
         <v>734</v>
       </c>
@@ -6125,7 +6174,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46">
       <c r="A46" t="s">
         <v>806</v>
       </c>
@@ -6184,7 +6233,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47">
       <c r="A47" t="s">
         <v>896</v>
       </c>
@@ -6243,7 +6292,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48">
       <c r="A48" t="s">
         <v>372</v>
       </c>
@@ -6296,7 +6345,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49">
       <c r="A49" t="s">
         <v>510</v>
       </c>
@@ -6349,7 +6398,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50">
       <c r="A50" t="s">
         <v>218</v>
       </c>
@@ -6402,7 +6451,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51">
       <c r="A51" t="s">
         <v>230</v>
       </c>
@@ -6455,7 +6504,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52">
       <c r="A52" t="s">
         <v>242</v>
       </c>
@@ -6508,7 +6557,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53">
       <c r="A53" t="s">
         <v>325</v>
       </c>
@@ -6561,7 +6610,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54">
       <c r="A54" t="s">
         <v>881</v>
       </c>
@@ -6617,7 +6666,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55">
       <c r="A55" t="s">
         <v>941</v>
       </c>
@@ -6673,7 +6722,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56">
       <c r="A56" t="s">
         <v>926</v>
       </c>
@@ -6729,7 +6778,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57">
       <c r="A57" t="s">
         <v>384</v>
       </c>
@@ -6782,7 +6831,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58">
       <c r="A58" t="s">
         <v>497</v>
       </c>
@@ -6835,7 +6884,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59">
       <c r="A59" t="s">
         <v>1001</v>
       </c>
@@ -6891,7 +6940,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60">
       <c r="A60" t="s">
         <v>523</v>
       </c>
@@ -6944,7 +6993,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61">
       <c r="A61" t="s">
         <v>675</v>
       </c>
@@ -7000,7 +7049,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62">
       <c r="A62" t="s">
         <v>576</v>
       </c>
@@ -7053,7 +7102,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63">
       <c r="A63" t="s">
         <v>719</v>
       </c>
@@ -7109,7 +7158,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64">
       <c r="A64" t="s">
         <v>866</v>
       </c>
@@ -7165,7 +7214,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65">
       <c r="A65" t="s">
         <v>1016</v>
       </c>
@@ -7221,7 +7270,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66">
       <c r="A66" t="s">
         <v>777</v>
       </c>
@@ -7277,7 +7326,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67">
       <c r="A67" t="s">
         <v>562</v>
       </c>
@@ -7330,7 +7379,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -7380,7 +7429,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69">
       <c r="A69" t="s">
         <v>704</v>
       </c>
@@ -7436,7 +7485,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -7486,7 +7535,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71">
       <c r="A71" t="s">
         <v>313</v>
       </c>
@@ -7539,7 +7588,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72">
       <c r="A72" t="s">
         <v>45</v>
       </c>
@@ -7589,7 +7638,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73">
       <c r="A73" t="s">
         <v>690</v>
       </c>
@@ -7642,7 +7691,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74">
       <c r="A74" t="s">
         <v>536</v>
       </c>
@@ -7695,7 +7744,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75">
       <c r="A75" t="s">
         <v>444</v>
       </c>
@@ -7748,7 +7797,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -7801,7 +7850,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77">
       <c r="A77" t="s">
         <v>134</v>
       </c>
@@ -7854,7 +7903,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78">
       <c r="A78" t="s">
         <v>194</v>
       </c>
@@ -7907,7 +7956,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79">
       <c r="A79" t="s">
         <v>971</v>
       </c>
@@ -7963,7 +8012,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80">
       <c r="A80" t="s">
         <v>986</v>
       </c>
@@ -8019,7 +8068,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81">
       <c r="A81" t="s">
         <v>956</v>
       </c>
@@ -8075,7 +8124,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82">
       <c r="A82" t="s">
         <v>432</v>
       </c>
@@ -8128,7 +8177,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83">
       <c r="A83" t="s">
         <v>1045</v>
       </c>
@@ -8185,7 +8234,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T83">
+  <sortState ref="A2:T83">
     <sortCondition ref="A2:A83"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
adding phase lock association
</commit_message>
<xml_diff>
--- a/config/becExpConfig/becExpType.csv.xlsx
+++ b/config/becExpConfig/becExpType.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weld Lab User\Documents\MMUser\config\becExpConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WOODHOUSE\Documents\MMUser\config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCB21F2-CC93-421D-8955-392F383D2C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D116D8D-EAD1-4468-8863-5B9B1AB26BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>TrialName</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Absorption</t>
+  </si>
+  <si>
+    <t>PhaseLockAssociation</t>
+  </si>
+  <si>
+    <t>WaveformAssociation</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,9 +487,10 @@
     <col min="16" max="16" width="16.42578125" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
     <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,8 +545,14 @@
       <c r="R1" t="s">
         <v>25</v>
       </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -593,6 +606,12 @@
       </c>
       <c r="R2" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start to work on atom number fit
</commit_message>
<xml_diff>
--- a/config/becExpConfig/becExpType.csv.xlsx
+++ b/config/becExpConfig/becExpType.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WOODHOUSE\Documents\MMUser\config\becExpConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7DD17-8DED-4213-8894-FFF740FA84A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AB94E0-4BC3-432C-9F7B-A24EDABAF5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="1198">
   <si>
     <t>TrialName</t>
   </si>
@@ -3020,6 +3020,426 @@
     <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingHf</t>
   </si>
   <si>
+    <t>OdtPainting</t>
+  </si>
+  <si>
+    <t>An experiment at ODT stage.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>AtomNumber;DensityFit;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[587 1430;820 1077;1185 1116;1412 1467;1386 1938;983 2154;629 1963;523 1643;509 1643]</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>NiBecTau</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting BEC stage. Scan tau.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[883 1331;920 1373;977 1409;1044 1385;1079 1289;1076 1226;1060 1180;1016 1173;953 1169;903 1189;878 1246]</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>ParabolicFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
+  </si>
+  <si>
+    <t>EvapDCameraSBB</t>
+  </si>
+  <si>
+    <t>An experiment at evaporation stage D.</t>
+  </si>
+  <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>CiceroLogTime</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>OdtCameraSBB</t>
+  </si>
+  <si>
+    <t>An experiment at ODT stage. Imaging along the lattice axis.</t>
+  </si>
+  <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>RunIndex</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>HfBecCameraSBB</t>
+  </si>
+  <si>
+    <t>An experiment at the high-field BEC stage.</t>
+  </si>
+  <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>RunIndex</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingHf</t>
+  </si>
+  <si>
+    <t>NiBecCameraSBB</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting BEC stage. Use the SBB (lattice) camera.</t>
+  </si>
+  <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>RunIndex</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[350 857;401 884;483 852;481 788;422 758;342 791]</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>ParabolicFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
+  </si>
+  <si>
+    <t>NiBecTofCameraOdt</t>
+  </si>
+  <si>
+    <t>A TOF experiment at the non-interacting BEC stage.</t>
+  </si>
+  <si>
+    <t>ODT</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>TOF</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[907 1249;924 1587;967 1593;1073 1593;1073 1468;1067 1326;1060 1215;1017 1158;918 1162]</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>ParabolicFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
+  </si>
+  <si>
+    <t>WaveformAssociation</t>
+  </si>
+  <si>
+    <t>PhaseLockAssociation</t>
+  </si>
+  <si>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingLf</t>
+  </si>
+  <si>
+    <t>NiBec</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting BEC stage.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>RunIndex</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>[883 1331;920 1373;977 1409;1044 1385;1079 1289;1076 1226;1060 1180;1016 1173;953 1169;903 1189;878 1246]</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>ParabolicFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
+  </si>
+  <si>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingNi</t>
+  </si>
+  <si>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingHf</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>A general test.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>CiceroLogTime</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>[450 1588;1338 859;1378 2311]</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>EvapD</t>
   </si>
   <si>
@@ -3065,10 +3485,16 @@
     <t>StdErr</t>
   </si>
   <si>
-    <t>OdtPainting</t>
-  </si>
-  <si>
-    <t>An experiment at ODT stage.</t>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingLf</t>
+  </si>
+  <si>
+    <t>AtomNumberFitMethod</t>
+  </si>
+  <si>
+    <t>EvapDIMCDetuning</t>
+  </si>
+  <si>
+    <t>An experiment at evaporation stage D. Scan IMC frequency.</t>
   </si>
   <si>
     <t>TOP</t>
@@ -3077,21 +3503,60 @@
     <t>EvapDOdt1</t>
   </si>
   <si>
+    <t>IMCDetuning</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>AtomNumber;DensityFit;CenterFit</t>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>StdErr</t>
+  </si>
+  <si>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingLf</t>
+  </si>
+  <si>
+    <t>EvapDIMCDetuning</t>
+  </si>
+  <si>
+    <t>An experiment at evaporation stage D. Scan IMC frequency.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>IMCDetuning</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
   </si>
   <si>
     <t>LSR</t>
   </si>
   <si>
-    <t>[587 1430;820 1077;1185 1116;1412 1467;1386 1938;983 2154;629 1963;523 1643;509 1643]</t>
-  </si>
-  <si>
     <t>LF</t>
   </si>
   <si>
@@ -3104,466 +3569,52 @@
     <t>BosonicGaussianFit1D</t>
   </si>
   <si>
+    <t>GaussianFit1D</t>
+  </si>
+  <si>
     <t>LinearFit1D</t>
   </si>
   <si>
     <t>StdErr</t>
   </si>
   <si>
-    <t>NiBecTau</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting BEC stage. Scan tau.</t>
+    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingLf</t>
+  </si>
+  <si>
+    <t>EvapDIMCDetuning</t>
+  </si>
+  <si>
+    <t>An experiment at evaporation stage D. Scan IMC frequency.</t>
   </si>
   <si>
     <t>TOP</t>
   </si>
   <si>
-    <t>Bec</t>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>IMCDetuning</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Absorption</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>tau</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>[883 1331;920 1373;977 1409;1044 1385;1079 1289;1076 1226;1060 1180;1016 1173;953 1169;903 1189;878 1246]</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>ParabolicFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
-  </si>
-  <si>
-    <t>EvapDCameraSBB</t>
-  </si>
-  <si>
-    <t>An experiment at evaporation stage D.</t>
-  </si>
-  <si>
-    <t>SBB</t>
-  </si>
-  <si>
-    <t>BecCameraSBB</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>CiceroLogTime</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>RandomPolarization</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>OdtCameraSBB</t>
-  </si>
-  <si>
-    <t>An experiment at ODT stage. Imaging along the lattice axis.</t>
-  </si>
-  <si>
-    <t>SBB</t>
-  </si>
-  <si>
-    <t>BecCameraSBB</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>RunIndex</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>RandomPolarization</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>HfBecCameraSBB</t>
-  </si>
-  <si>
-    <t>An experiment at the high-field BEC stage.</t>
-  </si>
-  <si>
-    <t>SBB</t>
-  </si>
-  <si>
-    <t>BecCameraSBB</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>RunIndex</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>RandomPolarization</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingHf</t>
-  </si>
-  <si>
-    <t>NiBecCameraSBB</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting BEC stage. Use the SBB (lattice) camera.</t>
-  </si>
-  <si>
-    <t>SBB</t>
-  </si>
-  <si>
-    <t>BecCameraSBB</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>RunIndex</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>[350 857;401 884;483 852;481 788;422 758;342 791]</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>RandomPolarization</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>ParabolicFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
-  </si>
-  <si>
-    <t>NiBecTofCameraOdt</t>
-  </si>
-  <si>
-    <t>A TOF experiment at the non-interacting BEC stage.</t>
-  </si>
-  <si>
-    <t>ODT</t>
-  </si>
-  <si>
-    <t>SideOdtCamera</t>
-  </si>
-  <si>
-    <t>TOF</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>[907 1249;924 1587;967 1593;1073 1593;1073 1468;1067 1326;1060 1215;1017 1158;918 1162]</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>ParabolicFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
-  </si>
-  <si>
-    <t>WaveformAssociation</t>
-  </si>
-  <si>
-    <t>PhaseLockAssociation</t>
-  </si>
-  <si>
-    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingLf</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>A general test.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>Full</t>
-  </si>
-  <si>
-    <t>CiceroLogTime</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>[450 1588;1338 859;1378 2311]</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>NiBec</t>
-  </si>
-  <si>
-    <t>An experiment at the non-interacting BEC stage.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>Bec</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>RunIndex</t>
-  </si>
-  <si>
-    <t>DensityFit;AtomNumber;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>[883 1331;920 1373;977 1409;1044 1385;1079 1289;1076 1226;1060 1180;1016 1173;953 1169;903 1189;878 1246]</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>ParabolicFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>WaveformGeneratorName,XvWingMod;ChannelName,Ch1;WaveformListName,XvWingNi</t>
-  </si>
-  <si>
-    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingNi</t>
-  </si>
-  <si>
-    <t>PhaseLockName,ImagingLock;Frequency,700000000;VariableName,hw_ImagingHf</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>A general test.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>Full</t>
-  </si>
-  <si>
-    <t>CiceroLogTime</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>[450 1588;1338 859;1378 2311]</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>StrongLight</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
-  </si>
-  <si>
-    <t>LinearFit1D</t>
-  </si>
-  <si>
-    <t>StdErr</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>EvapD</t>
-  </si>
-  <si>
-    <t>An experiment at evaporation stage D.</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>EvapDOdt1</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>CiceroLogTime</t>
-  </si>
-  <si>
-    <t>AtomNumber;DensityFit;CenterFit</t>
-  </si>
-  <si>
-    <t>LSR</t>
-  </si>
-  <si>
-    <t>[549 1745;903 1905;1286 1930;1532 1678;1603 1325;1617 1085;1501 850;1355 743;908 715;693 740;535 925;522 1284]</t>
-  </si>
-  <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>Absorption</t>
-  </si>
-  <si>
-    <t>RandomPolarization</t>
-  </si>
-  <si>
-    <t>BosonicGaussianFit1D</t>
   </si>
   <si>
     <t>LinearFit1D</t>
@@ -3899,10 +3950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U86"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="true" topLeftCell="J57" workbookViewId="0">
+      <selection activeCell="Q88" sqref="Q88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3923,11 +3974,12 @@
     <col min="14" max="14" width="7.85546875" customWidth="true"/>
     <col min="15" max="15" width="20.42578125" customWidth="true"/>
     <col min="16" max="16" width="17.42578125" customWidth="true"/>
-    <col min="17" max="17" width="16.42578125" customWidth="true"/>
-    <col min="18" max="18" width="17" customWidth="true"/>
-    <col min="19" max="19" width="16.85546875" customWidth="true"/>
-    <col min="20" max="20" width="84.28515625" customWidth="true"/>
-    <col min="21" max="21" width="73" customWidth="true"/>
+    <col min="17" max="17" width="22.5703125" customWidth="true"/>
+    <col min="18" max="18" width="16.42578125" customWidth="true"/>
+    <col min="19" max="19" width="17" customWidth="true"/>
+    <col min="20" max="20" width="16.85546875" customWidth="true"/>
+    <col min="21" max="21" width="84.28515625" customWidth="true"/>
+    <col min="22" max="22" width="73" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3980,19 +4032,22 @@
         <v>11</v>
       </c>
       <c r="Q1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>420</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>539</v>
       </c>
-      <c r="T1" t="s">
-        <v>1116</v>
-      </c>
       <c r="U1" t="s">
-        <v>1117</v>
+        <v>1101</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="2">
@@ -4036,13 +4091,16 @@
         <v>30</v>
       </c>
       <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
         <v>67</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>421</v>
       </c>
-      <c r="U2" t="s">
-        <v>1118</v>
+      <c r="V2" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="3">
@@ -4086,74 +4144,78 @@
         <v>30</v>
       </c>
       <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
         <v>33</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>421</v>
       </c>
-      <c r="U3" t="s">
-        <v>1118</v>
+      <c r="V3" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>1168</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>1169</v>
-      </c>
-      <c r="F4" s="0">
+      <c r="A4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>1170</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>1171</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>1175</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>1176</v>
-      </c>
-      <c r="N4" s="0">
+      <c r="G4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N4">
         <v>8</v>
       </c>
-      <c r="O4" s="0" t="s">
-        <v>1177</v>
-      </c>
-      <c r="P4" s="0">
+      <c r="O4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="P4">
         <v>40</v>
       </c>
-      <c r="Q4" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="S4" s="0"/>
-      <c r="T4" s="0"/>
-      <c r="U4" s="0" t="s">
-        <v>1180</v>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="V4" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="5">
@@ -4203,69 +4265,75 @@
         <v>30</v>
       </c>
       <c r="Q5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
         <v>371</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>421</v>
       </c>
-      <c r="U5" t="s">
-        <v>1118</v>
+      <c r="V5" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>1042</v>
+        <v>1027</v>
       </c>
       <c r="B6" t="s">
-        <v>1043</v>
+        <v>1028</v>
       </c>
       <c r="C6" t="s">
-        <v>1044</v>
+        <v>1029</v>
       </c>
       <c r="D6" t="s">
-        <v>1045</v>
+        <v>1030</v>
       </c>
       <c r="E6" t="s">
-        <v>1046</v>
+        <v>1031</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>1047</v>
+        <v>1032</v>
       </c>
       <c r="H6" t="s">
-        <v>1048</v>
+        <v>1033</v>
       </c>
       <c r="I6" t="s">
-        <v>1049</v>
+        <v>1034</v>
       </c>
       <c r="K6" t="s">
-        <v>1050</v>
+        <v>1035</v>
       </c>
       <c r="L6" t="s">
-        <v>1051</v>
+        <v>1036</v>
       </c>
       <c r="M6" t="s">
-        <v>1052</v>
+        <v>1037</v>
       </c>
       <c r="N6">
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>1053</v>
+        <v>1038</v>
       </c>
       <c r="P6">
         <v>30</v>
       </c>
       <c r="Q6" t="s">
-        <v>1054</v>
+        <v>19</v>
       </c>
       <c r="R6" t="s">
-        <v>1055</v>
-      </c>
-      <c r="U6" t="s">
-        <v>1118</v>
+        <v>1039</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="7">
@@ -4312,13 +4380,16 @@
         <v>30</v>
       </c>
       <c r="Q7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" t="s">
         <v>88</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>421</v>
       </c>
-      <c r="U7" t="s">
-        <v>1118</v>
+      <c r="V7" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="8">
@@ -4368,13 +4439,16 @@
         <v>30</v>
       </c>
       <c r="Q8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" t="s">
         <v>623</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>624</v>
       </c>
-      <c r="U8" t="s">
-        <v>1118</v>
+      <c r="V8" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="9">
@@ -4424,66 +4498,76 @@
         <v>30</v>
       </c>
       <c r="Q9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" t="s">
         <v>383</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>421</v>
       </c>
-      <c r="U9" t="s">
-        <v>1118</v>
+      <c r="V9" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10">
+      <c r="A10" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" t="s">
-        <v>95</v>
-      </c>
-      <c r="K10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L10" t="s">
-        <v>580</v>
-      </c>
-      <c r="M10" t="s">
-        <v>97</v>
-      </c>
-      <c r="N10">
+      <c r="G10" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="N10" s="0">
         <v>8</v>
       </c>
-      <c r="O10" t="s">
-        <v>98</v>
-      </c>
-      <c r="P10">
+      <c r="O10" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="P10" s="0">
         <v>30</v>
       </c>
-      <c r="Q10" t="s">
-        <v>99</v>
-      </c>
-      <c r="R10" t="s">
-        <v>421</v>
-      </c>
-      <c r="U10" t="s">
-        <v>1118</v>
+      <c r="Q10" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0" t="s">
+        <v>1197</v>
       </c>
     </row>
     <row r="11">
@@ -4533,13 +4617,16 @@
         <v>30</v>
       </c>
       <c r="Q11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" t="s">
         <v>395</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>421</v>
       </c>
-      <c r="U11" t="s">
-        <v>1118</v>
+      <c r="V11" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="12">
@@ -4589,13 +4676,16 @@
         <v>30</v>
       </c>
       <c r="Q12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" t="s">
         <v>133</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>421</v>
       </c>
-      <c r="U12" t="s">
-        <v>1118</v>
+      <c r="V12" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="13">
@@ -4645,13 +4735,16 @@
         <v>30</v>
       </c>
       <c r="Q13" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" t="s">
         <v>217</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>421</v>
       </c>
-      <c r="U13" t="s">
-        <v>1118</v>
+      <c r="V13" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="14">
@@ -4701,13 +4794,16 @@
         <v>40</v>
       </c>
       <c r="Q14" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" t="s">
         <v>594</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>595</v>
       </c>
-      <c r="U14" t="s">
-        <v>1118</v>
+      <c r="V14" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="15">
@@ -4754,13 +4850,16 @@
         <v>30</v>
       </c>
       <c r="Q15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" t="s">
         <v>44</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>421</v>
       </c>
-      <c r="U15" t="s">
-        <v>1118</v>
+      <c r="V15" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="16">
@@ -4804,13 +4903,16 @@
         <v>30</v>
       </c>
       <c r="Q16" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" t="s">
         <v>23</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>421</v>
       </c>
-      <c r="U16" t="s">
-        <v>1118</v>
+      <c r="V16" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="17">
@@ -4860,75 +4962,81 @@
         <v>2</v>
       </c>
       <c r="Q17" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" t="s">
         <v>993</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>994</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>995</v>
       </c>
-      <c r="U17" t="s">
-        <v>1150</v>
+      <c r="V17" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="B18" t="s">
-        <v>1071</v>
+        <v>1056</v>
       </c>
       <c r="C18" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="D18" t="s">
-        <v>1073</v>
+        <v>1058</v>
       </c>
       <c r="E18" t="s">
-        <v>1074</v>
+        <v>1059</v>
       </c>
       <c r="F18">
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>1075</v>
+        <v>1060</v>
       </c>
       <c r="H18" t="s">
-        <v>1076</v>
+        <v>1061</v>
       </c>
       <c r="I18" t="s">
-        <v>1077</v>
+        <v>1062</v>
       </c>
       <c r="K18" t="s">
-        <v>1078</v>
+        <v>1063</v>
       </c>
       <c r="L18" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="M18" t="s">
-        <v>1080</v>
+        <v>1065</v>
       </c>
       <c r="N18">
         <v>8</v>
       </c>
       <c r="O18" t="s">
-        <v>1081</v>
+        <v>1066</v>
       </c>
       <c r="P18">
         <v>2</v>
       </c>
       <c r="Q18" t="s">
-        <v>1082</v>
+        <v>19</v>
       </c>
       <c r="R18" t="s">
-        <v>1083</v>
-      </c>
-      <c r="T18" t="s">
-        <v>1084</v>
+        <v>1067</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1068</v>
       </c>
       <c r="U18" t="s">
-        <v>1150</v>
+        <v>1069</v>
+      </c>
+      <c r="V18" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="19">
@@ -4978,16 +5086,19 @@
         <v>2</v>
       </c>
       <c r="Q19" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" t="s">
         <v>323</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>421</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>995</v>
       </c>
-      <c r="U19" t="s">
-        <v>1150</v>
+      <c r="V19" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="20">
@@ -5040,16 +5151,19 @@
         <v>2</v>
       </c>
       <c r="Q20" t="s">
+        <v>19</v>
+      </c>
+      <c r="R20" t="s">
         <v>609</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>610</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>995</v>
       </c>
-      <c r="U20" t="s">
-        <v>1150</v>
+      <c r="V20" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="21">
@@ -5102,16 +5216,19 @@
         <v>2</v>
       </c>
       <c r="Q21" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" t="s">
         <v>858</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>859</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>995</v>
       </c>
-      <c r="U21" t="s">
-        <v>1150</v>
+      <c r="V21" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="22">
@@ -5161,16 +5278,19 @@
         <v>2</v>
       </c>
       <c r="Q22" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22" t="s">
         <v>459</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>460</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>995</v>
       </c>
-      <c r="U22" t="s">
-        <v>1150</v>
+      <c r="V22" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="23">
@@ -5220,16 +5340,19 @@
         <v>2</v>
       </c>
       <c r="Q23" t="s">
+        <v>19</v>
+      </c>
+      <c r="R23" t="s">
         <v>288</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>421</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>995</v>
       </c>
-      <c r="U23" t="s">
-        <v>1150</v>
+      <c r="V23" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="24">
@@ -5279,16 +5402,19 @@
         <v>2</v>
       </c>
       <c r="Q24" t="s">
+        <v>19</v>
+      </c>
+      <c r="R24" t="s">
         <v>446</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>447</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>995</v>
       </c>
-      <c r="U24" t="s">
-        <v>1150</v>
+      <c r="V24" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="25">
@@ -5338,16 +5464,19 @@
         <v>2</v>
       </c>
       <c r="Q25" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" t="s">
         <v>524</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>525</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>995</v>
       </c>
-      <c r="U25" t="s">
-        <v>1150</v>
+      <c r="V25" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="26">
@@ -5397,16 +5526,19 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
+        <v>19</v>
+      </c>
+      <c r="R26" t="s">
         <v>977</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>978</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>995</v>
       </c>
-      <c r="U26" t="s">
-        <v>1150</v>
+      <c r="V26" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="27">
@@ -5453,13 +5585,16 @@
         <v>30</v>
       </c>
       <c r="Q27" t="s">
+        <v>19</v>
+      </c>
+      <c r="R27" t="s">
         <v>264</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>421</v>
       </c>
-      <c r="U27" t="s">
-        <v>1118</v>
+      <c r="V27" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="28">
@@ -5506,13 +5641,16 @@
         <v>30</v>
       </c>
       <c r="Q28" t="s">
+        <v>19</v>
+      </c>
+      <c r="R28" t="s">
         <v>311</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>421</v>
       </c>
-      <c r="U28" t="s">
-        <v>1118</v>
+      <c r="V28" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="29">
@@ -5559,75 +5697,81 @@
         <v>30</v>
       </c>
       <c r="Q29" t="s">
+        <v>19</v>
+      </c>
+      <c r="R29" t="s">
         <v>121</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>421</v>
       </c>
-      <c r="U29" t="s">
-        <v>1118</v>
+      <c r="V29" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>1133</v>
+        <v>1104</v>
       </c>
       <c r="B30" t="s">
-        <v>1134</v>
+        <v>1105</v>
       </c>
       <c r="C30" t="s">
-        <v>1135</v>
+        <v>1106</v>
       </c>
       <c r="D30" t="s">
-        <v>1136</v>
+        <v>1107</v>
       </c>
       <c r="E30" t="s">
-        <v>1137</v>
+        <v>1108</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>1138</v>
+        <v>1109</v>
       </c>
       <c r="H30" t="s">
-        <v>1139</v>
+        <v>1110</v>
       </c>
       <c r="I30" t="s">
-        <v>1140</v>
+        <v>1111</v>
       </c>
       <c r="J30" t="s">
-        <v>1141</v>
+        <v>1112</v>
       </c>
       <c r="K30" t="s">
-        <v>1142</v>
+        <v>1113</v>
       </c>
       <c r="L30" t="s">
-        <v>1143</v>
+        <v>1114</v>
       </c>
       <c r="M30" t="s">
-        <v>1144</v>
+        <v>1115</v>
       </c>
       <c r="N30">
         <v>8</v>
       </c>
       <c r="O30" t="s">
-        <v>1145</v>
+        <v>1116</v>
       </c>
       <c r="P30">
         <v>0.2</v>
       </c>
       <c r="Q30" t="s">
-        <v>1146</v>
+        <v>19</v>
       </c>
       <c r="R30" t="s">
-        <v>1147</v>
-      </c>
-      <c r="T30" t="s">
-        <v>1148</v>
+        <v>1117</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1118</v>
       </c>
       <c r="U30" t="s">
-        <v>1149</v>
+        <v>1119</v>
+      </c>
+      <c r="V30" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="31">
@@ -5677,78 +5821,84 @@
         <v>0.2</v>
       </c>
       <c r="Q31" t="s">
+        <v>19</v>
+      </c>
+      <c r="R31" t="s">
         <v>335</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>421</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>979</v>
       </c>
-      <c r="U31" t="s">
-        <v>1149</v>
+      <c r="V31" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1085</v>
+        <v>1070</v>
       </c>
       <c r="B32" t="s">
-        <v>1086</v>
+        <v>1071</v>
       </c>
       <c r="C32" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="D32" t="s">
-        <v>1088</v>
+        <v>1073</v>
       </c>
       <c r="E32" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="F32">
         <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="H32" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="I32" t="s">
-        <v>1092</v>
+        <v>1077</v>
       </c>
       <c r="J32" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="K32" t="s">
-        <v>1094</v>
+        <v>1079</v>
       </c>
       <c r="L32" t="s">
-        <v>1095</v>
+        <v>1080</v>
       </c>
       <c r="M32" t="s">
-        <v>1096</v>
+        <v>1081</v>
       </c>
       <c r="N32">
         <v>20</v>
       </c>
       <c r="O32" t="s">
-        <v>1097</v>
+        <v>1082</v>
       </c>
       <c r="P32">
         <v>0.2</v>
       </c>
       <c r="Q32" t="s">
-        <v>1098</v>
+        <v>19</v>
       </c>
       <c r="R32" t="s">
-        <v>1099</v>
-      </c>
-      <c r="T32" t="s">
-        <v>1100</v>
+        <v>1083</v>
+      </c>
+      <c r="S32" t="s">
+        <v>1084</v>
       </c>
       <c r="U32" t="s">
-        <v>1149</v>
+        <v>1085</v>
+      </c>
+      <c r="V32" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="33">
@@ -5798,16 +5948,19 @@
         <v>10</v>
       </c>
       <c r="Q33" t="s">
+        <v>19</v>
+      </c>
+      <c r="R33" t="s">
         <v>181</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>421</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>979</v>
       </c>
-      <c r="U33" t="s">
-        <v>1149</v>
+      <c r="V33" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="34">
@@ -5857,16 +6010,19 @@
         <v>0.2</v>
       </c>
       <c r="Q34" t="s">
+        <v>19</v>
+      </c>
+      <c r="R34" t="s">
         <v>724</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>725</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>979</v>
       </c>
-      <c r="U34" t="s">
-        <v>1149</v>
+      <c r="V34" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="35">
@@ -5919,16 +6075,19 @@
         <v>0.5</v>
       </c>
       <c r="Q35" t="s">
+        <v>19</v>
+      </c>
+      <c r="R35" t="s">
         <v>783</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>784</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>979</v>
       </c>
-      <c r="U35" t="s">
-        <v>1149</v>
+      <c r="V35" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="36">
@@ -5978,16 +6137,19 @@
         <v>0.2</v>
       </c>
       <c r="Q36" t="s">
+        <v>19</v>
+      </c>
+      <c r="R36" t="s">
         <v>276</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>421</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>979</v>
       </c>
-      <c r="U36" t="s">
-        <v>1149</v>
+      <c r="V36" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="37">
@@ -6037,16 +6199,19 @@
         <v>1</v>
       </c>
       <c r="Q37" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" t="s">
         <v>193</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>421</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>979</v>
       </c>
-      <c r="U37" t="s">
-        <v>1149</v>
+      <c r="V37" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="38">
@@ -6099,16 +6264,19 @@
         <v>0.2</v>
       </c>
       <c r="Q38" t="s">
+        <v>19</v>
+      </c>
+      <c r="R38" t="s">
         <v>798</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>799</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>979</v>
       </c>
-      <c r="U38" t="s">
-        <v>1149</v>
+      <c r="V38" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="39">
@@ -6158,16 +6326,19 @@
         <v>0.2</v>
       </c>
       <c r="Q39" t="s">
+        <v>19</v>
+      </c>
+      <c r="R39" t="s">
         <v>433</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>434</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>979</v>
       </c>
-      <c r="U39" t="s">
-        <v>1149</v>
+      <c r="V39" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="40">
@@ -6217,16 +6388,19 @@
         <v>0.2</v>
       </c>
       <c r="Q40" t="s">
+        <v>19</v>
+      </c>
+      <c r="R40" t="s">
         <v>577</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>578</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>979</v>
       </c>
-      <c r="U40" t="s">
-        <v>1149</v>
+      <c r="V40" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="41">
@@ -6276,16 +6450,19 @@
         <v>1</v>
       </c>
       <c r="Q41" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" t="s">
         <v>637</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>638</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>979</v>
       </c>
-      <c r="U41" t="s">
-        <v>1149</v>
+      <c r="V41" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="42">
@@ -6335,16 +6512,19 @@
         <v>0.2</v>
       </c>
       <c r="Q42" t="s">
+        <v>19</v>
+      </c>
+      <c r="R42" t="s">
         <v>564</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>565</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
         <v>979</v>
       </c>
-      <c r="U42" t="s">
-        <v>1149</v>
+      <c r="V42" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="43">
@@ -6394,16 +6574,19 @@
         <v>0.2</v>
       </c>
       <c r="Q43" t="s">
+        <v>19</v>
+      </c>
+      <c r="R43" t="s">
         <v>753</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>754</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>979</v>
       </c>
-      <c r="U43" t="s">
-        <v>1149</v>
+      <c r="V43" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="44">
@@ -6453,16 +6636,19 @@
         <v>0.2</v>
       </c>
       <c r="Q44" t="s">
+        <v>19</v>
+      </c>
+      <c r="R44" t="s">
         <v>169</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>421</v>
       </c>
-      <c r="T44" t="s">
+      <c r="U44" t="s">
         <v>979</v>
       </c>
-      <c r="U44" t="s">
-        <v>1149</v>
+      <c r="V44" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="45">
@@ -6512,16 +6698,19 @@
         <v>0.2</v>
       </c>
       <c r="Q45" t="s">
+        <v>19</v>
+      </c>
+      <c r="R45" t="s">
         <v>710</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>711</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>980</v>
       </c>
-      <c r="U45" t="s">
-        <v>1149</v>
+      <c r="V45" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="46">
@@ -6574,16 +6763,19 @@
         <v>0.2</v>
       </c>
       <c r="Q46" t="s">
+        <v>19</v>
+      </c>
+      <c r="R46" t="s">
         <v>768</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>769</v>
       </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
         <v>980</v>
       </c>
-      <c r="U46" t="s">
-        <v>1149</v>
+      <c r="V46" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="47">
@@ -6636,16 +6828,19 @@
         <v>0.2</v>
       </c>
       <c r="Q47" t="s">
+        <v>19</v>
+      </c>
+      <c r="R47" t="s">
         <v>843</v>
       </c>
-      <c r="R47" t="s">
+      <c r="S47" t="s">
         <v>844</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
         <v>980</v>
       </c>
-      <c r="U47" t="s">
-        <v>1149</v>
+      <c r="V47" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="48">
@@ -6695,13 +6890,16 @@
         <v>0.2</v>
       </c>
       <c r="Q48" t="s">
+        <v>19</v>
+      </c>
+      <c r="R48" t="s">
         <v>347</v>
       </c>
-      <c r="R48" t="s">
+      <c r="S48" t="s">
         <v>421</v>
       </c>
-      <c r="U48" t="s">
-        <v>1149</v>
+      <c r="V48" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="49">
@@ -6751,13 +6949,16 @@
         <v>0.2</v>
       </c>
       <c r="Q49" t="s">
+        <v>19</v>
+      </c>
+      <c r="R49" t="s">
         <v>485</v>
       </c>
-      <c r="R49" t="s">
+      <c r="S49" t="s">
         <v>486</v>
       </c>
-      <c r="U49" t="s">
-        <v>1149</v>
+      <c r="V49" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="50">
@@ -6807,13 +7008,16 @@
         <v>1</v>
       </c>
       <c r="Q50" t="s">
+        <v>19</v>
+      </c>
+      <c r="R50" t="s">
         <v>229</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>421</v>
       </c>
-      <c r="U50" t="s">
-        <v>1149</v>
+      <c r="V50" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="51">
@@ -6863,13 +7067,16 @@
         <v>0.2</v>
       </c>
       <c r="Q51" t="s">
+        <v>19</v>
+      </c>
+      <c r="R51" t="s">
         <v>241</v>
       </c>
-      <c r="R51" t="s">
+      <c r="S51" t="s">
         <v>421</v>
       </c>
-      <c r="U51" t="s">
-        <v>1149</v>
+      <c r="V51" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="52">
@@ -6919,13 +7126,16 @@
         <v>0.2</v>
       </c>
       <c r="Q52" t="s">
+        <v>19</v>
+      </c>
+      <c r="R52" t="s">
         <v>253</v>
       </c>
-      <c r="R52" t="s">
+      <c r="S52" t="s">
         <v>421</v>
       </c>
-      <c r="U52" t="s">
-        <v>1149</v>
+      <c r="V52" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="53">
@@ -6975,13 +7185,16 @@
         <v>0.2</v>
       </c>
       <c r="Q53" t="s">
+        <v>19</v>
+      </c>
+      <c r="R53" t="s">
         <v>300</v>
       </c>
-      <c r="R53" t="s">
+      <c r="S53" t="s">
         <v>421</v>
       </c>
-      <c r="U53" t="s">
-        <v>1149</v>
+      <c r="V53" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="54">
@@ -7034,13 +7247,16 @@
         <v>0.2</v>
       </c>
       <c r="Q54" t="s">
+        <v>19</v>
+      </c>
+      <c r="R54" t="s">
         <v>828</v>
       </c>
-      <c r="R54" t="s">
+      <c r="S54" t="s">
         <v>829</v>
       </c>
-      <c r="U54" t="s">
-        <v>1149</v>
+      <c r="V54" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="55">
@@ -7093,13 +7309,16 @@
         <v>0.2</v>
       </c>
       <c r="Q55" t="s">
+        <v>19</v>
+      </c>
+      <c r="R55" t="s">
         <v>888</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>889</v>
       </c>
-      <c r="U55" t="s">
-        <v>1149</v>
+      <c r="V55" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="56">
@@ -7152,13 +7371,16 @@
         <v>1</v>
       </c>
       <c r="Q56" t="s">
+        <v>19</v>
+      </c>
+      <c r="R56" t="s">
         <v>873</v>
       </c>
-      <c r="R56" t="s">
+      <c r="S56" t="s">
         <v>874</v>
       </c>
-      <c r="U56" t="s">
-        <v>1149</v>
+      <c r="V56" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="57">
@@ -7208,13 +7430,16 @@
         <v>1</v>
       </c>
       <c r="Q57" t="s">
+        <v>19</v>
+      </c>
+      <c r="R57" t="s">
         <v>359</v>
       </c>
-      <c r="R57" t="s">
+      <c r="S57" t="s">
         <v>421</v>
       </c>
-      <c r="U57" t="s">
-        <v>1149</v>
+      <c r="V57" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="58">
@@ -7264,13 +7489,16 @@
         <v>0.2</v>
       </c>
       <c r="Q58" t="s">
+        <v>19</v>
+      </c>
+      <c r="R58" t="s">
         <v>472</v>
       </c>
-      <c r="R58" t="s">
+      <c r="S58" t="s">
         <v>473</v>
       </c>
-      <c r="U58" t="s">
-        <v>1149</v>
+      <c r="V58" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="59">
@@ -7323,13 +7551,16 @@
         <v>0.2</v>
       </c>
       <c r="Q59" t="s">
+        <v>19</v>
+      </c>
+      <c r="R59" t="s">
         <v>948</v>
       </c>
-      <c r="R59" t="s">
+      <c r="S59" t="s">
         <v>949</v>
       </c>
-      <c r="U59" t="s">
-        <v>1149</v>
+      <c r="V59" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="60">
@@ -7379,13 +7610,16 @@
         <v>0.2</v>
       </c>
       <c r="Q60" t="s">
+        <v>19</v>
+      </c>
+      <c r="R60" t="s">
         <v>498</v>
       </c>
-      <c r="R60" t="s">
+      <c r="S60" t="s">
         <v>499</v>
       </c>
-      <c r="U60" t="s">
-        <v>1149</v>
+      <c r="V60" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="61">
@@ -7438,13 +7672,16 @@
         <v>0.2</v>
       </c>
       <c r="Q61" t="s">
+        <v>19</v>
+      </c>
+      <c r="R61" t="s">
         <v>652</v>
       </c>
-      <c r="R61" t="s">
+      <c r="S61" t="s">
         <v>653</v>
       </c>
-      <c r="U61" t="s">
-        <v>1149</v>
+      <c r="V61" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="62">
@@ -7494,13 +7731,16 @@
         <v>0.2</v>
       </c>
       <c r="Q62" t="s">
+        <v>19</v>
+      </c>
+      <c r="R62" t="s">
         <v>551</v>
       </c>
-      <c r="R62" t="s">
+      <c r="S62" t="s">
         <v>552</v>
       </c>
-      <c r="U62" t="s">
-        <v>1149</v>
+      <c r="V62" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="63">
@@ -7553,13 +7793,16 @@
         <v>0.2</v>
       </c>
       <c r="Q63" t="s">
+        <v>19</v>
+      </c>
+      <c r="R63" t="s">
         <v>696</v>
       </c>
-      <c r="R63" t="s">
+      <c r="S63" t="s">
         <v>697</v>
       </c>
-      <c r="U63" t="s">
-        <v>1149</v>
+      <c r="V63" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="64">
@@ -7612,13 +7855,16 @@
         <v>1</v>
       </c>
       <c r="Q64" t="s">
+        <v>19</v>
+      </c>
+      <c r="R64" t="s">
         <v>813</v>
       </c>
-      <c r="R64" t="s">
+      <c r="S64" t="s">
         <v>814</v>
       </c>
-      <c r="U64" t="s">
-        <v>1149</v>
+      <c r="V64" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="65">
@@ -7671,13 +7917,16 @@
         <v>0.2</v>
       </c>
       <c r="Q65" t="s">
+        <v>19</v>
+      </c>
+      <c r="R65" t="s">
         <v>963</v>
       </c>
-      <c r="R65" t="s">
+      <c r="S65" t="s">
         <v>964</v>
       </c>
-      <c r="U65" t="s">
-        <v>1149</v>
+      <c r="V65" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="66">
@@ -7730,13 +7979,16 @@
         <v>1</v>
       </c>
       <c r="Q66" t="s">
+        <v>19</v>
+      </c>
+      <c r="R66" t="s">
         <v>739</v>
       </c>
-      <c r="R66" t="s">
+      <c r="S66" t="s">
         <v>740</v>
       </c>
-      <c r="U66" t="s">
-        <v>1149</v>
+      <c r="V66" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="67">
@@ -7786,13 +8038,16 @@
         <v>0.2</v>
       </c>
       <c r="Q67" t="s">
+        <v>19</v>
+      </c>
+      <c r="R67" t="s">
         <v>537</v>
       </c>
-      <c r="R67" t="s">
+      <c r="S67" t="s">
         <v>538</v>
       </c>
-      <c r="U67" t="s">
-        <v>1149</v>
+      <c r="V67" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="68">
@@ -7839,13 +8094,16 @@
         <v>0.2</v>
       </c>
       <c r="Q68" t="s">
+        <v>19</v>
+      </c>
+      <c r="R68" t="s">
         <v>110</v>
       </c>
-      <c r="R68" t="s">
+      <c r="S68" t="s">
         <v>421</v>
       </c>
-      <c r="U68" t="s">
-        <v>1149</v>
+      <c r="V68" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="69">
@@ -7898,13 +8156,16 @@
         <v>15</v>
       </c>
       <c r="Q69" t="s">
+        <v>19</v>
+      </c>
+      <c r="R69" t="s">
         <v>681</v>
       </c>
-      <c r="R69" t="s">
+      <c r="S69" t="s">
         <v>682</v>
       </c>
-      <c r="U69" t="s">
-        <v>1118</v>
+      <c r="V69" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="70">
@@ -7951,69 +8212,75 @@
         <v>15</v>
       </c>
       <c r="Q70" t="s">
+        <v>19</v>
+      </c>
+      <c r="R70" t="s">
         <v>66</v>
       </c>
-      <c r="R70" t="s">
+      <c r="S70" t="s">
         <v>421</v>
       </c>
-      <c r="U70" t="s">
-        <v>1118</v>
+      <c r="V70" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>1056</v>
+        <v>1041</v>
       </c>
       <c r="B71" t="s">
-        <v>1057</v>
+        <v>1042</v>
       </c>
       <c r="C71" t="s">
-        <v>1058</v>
+        <v>1043</v>
       </c>
       <c r="D71" t="s">
-        <v>1059</v>
+        <v>1044</v>
       </c>
       <c r="E71" t="s">
-        <v>1060</v>
+        <v>1045</v>
       </c>
       <c r="F71">
         <v>4</v>
       </c>
       <c r="G71" t="s">
-        <v>1061</v>
+        <v>1046</v>
       </c>
       <c r="H71" t="s">
-        <v>1062</v>
+        <v>1047</v>
       </c>
       <c r="I71" t="s">
-        <v>1063</v>
+        <v>1048</v>
       </c>
       <c r="K71" t="s">
-        <v>1064</v>
+        <v>1049</v>
       </c>
       <c r="L71" t="s">
-        <v>1065</v>
+        <v>1050</v>
       </c>
       <c r="M71" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="N71">
         <v>8</v>
       </c>
       <c r="O71" t="s">
-        <v>1067</v>
+        <v>1052</v>
       </c>
       <c r="P71">
         <v>15</v>
       </c>
       <c r="Q71" t="s">
-        <v>1068</v>
+        <v>19</v>
       </c>
       <c r="R71" t="s">
-        <v>1069</v>
-      </c>
-      <c r="U71" t="s">
-        <v>1118</v>
+        <v>1053</v>
+      </c>
+      <c r="S71" t="s">
+        <v>1054</v>
+      </c>
+      <c r="V71" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="72">
@@ -8060,13 +8327,16 @@
         <v>15</v>
       </c>
       <c r="Q72" t="s">
+        <v>19</v>
+      </c>
+      <c r="R72" t="s">
         <v>55</v>
       </c>
-      <c r="R72" t="s">
+      <c r="S72" t="s">
         <v>421</v>
       </c>
-      <c r="U72" t="s">
-        <v>1118</v>
+      <c r="V72" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="73">
@@ -8116,13 +8386,16 @@
         <v>15</v>
       </c>
       <c r="Q73" t="s">
+        <v>19</v>
+      </c>
+      <c r="R73" t="s">
         <v>666</v>
       </c>
-      <c r="R73" t="s">
+      <c r="S73" t="s">
         <v>667</v>
       </c>
-      <c r="U73" t="s">
-        <v>1118</v>
+      <c r="V73" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="74">
@@ -8172,13 +8445,16 @@
         <v>15</v>
       </c>
       <c r="Q74" t="s">
+        <v>19</v>
+      </c>
+      <c r="R74" t="s">
         <v>511</v>
       </c>
-      <c r="R74" t="s">
+      <c r="S74" t="s">
         <v>512</v>
       </c>
-      <c r="U74" t="s">
-        <v>1118</v>
+      <c r="V74" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="75">
@@ -8228,13 +8504,16 @@
         <v>200</v>
       </c>
       <c r="Q75" t="s">
+        <v>19</v>
+      </c>
+      <c r="R75" t="s">
         <v>419</v>
       </c>
-      <c r="R75" t="s">
+      <c r="S75" t="s">
         <v>421</v>
       </c>
-      <c r="U75" t="s">
-        <v>1118</v>
+      <c r="V75" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="76">
@@ -8284,13 +8563,16 @@
         <v>30</v>
       </c>
       <c r="Q76" t="s">
+        <v>19</v>
+      </c>
+      <c r="R76" t="s">
         <v>157</v>
       </c>
-      <c r="R76" t="s">
+      <c r="S76" t="s">
         <v>421</v>
       </c>
-      <c r="U76" t="s">
-        <v>1118</v>
+      <c r="V76" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="77">
@@ -8340,13 +8622,16 @@
         <v>30</v>
       </c>
       <c r="Q77" t="s">
+        <v>19</v>
+      </c>
+      <c r="R77" t="s">
         <v>145</v>
       </c>
-      <c r="R77" t="s">
+      <c r="S77" t="s">
         <v>421</v>
       </c>
-      <c r="U77" t="s">
-        <v>1118</v>
+      <c r="V77" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="78">
@@ -8396,13 +8681,16 @@
         <v>30</v>
       </c>
       <c r="Q78" t="s">
+        <v>19</v>
+      </c>
+      <c r="R78" t="s">
         <v>205</v>
       </c>
-      <c r="R78" t="s">
+      <c r="S78" t="s">
         <v>421</v>
       </c>
-      <c r="U78" t="s">
-        <v>1118</v>
+      <c r="V78" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="79">
@@ -8455,13 +8743,16 @@
         <v>30</v>
       </c>
       <c r="Q79" t="s">
+        <v>19</v>
+      </c>
+      <c r="R79" t="s">
         <v>918</v>
       </c>
-      <c r="R79" t="s">
+      <c r="S79" t="s">
         <v>919</v>
       </c>
-      <c r="U79" t="s">
-        <v>1118</v>
+      <c r="V79" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="80">
@@ -8514,13 +8805,16 @@
         <v>30</v>
       </c>
       <c r="Q80" t="s">
+        <v>19</v>
+      </c>
+      <c r="R80" t="s">
         <v>933</v>
       </c>
-      <c r="R80" t="s">
+      <c r="S80" t="s">
         <v>934</v>
       </c>
-      <c r="U80" t="s">
-        <v>1118</v>
+      <c r="V80" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="81">
@@ -8573,13 +8867,16 @@
         <v>15</v>
       </c>
       <c r="Q81" t="s">
+        <v>19</v>
+      </c>
+      <c r="R81" t="s">
         <v>903</v>
       </c>
-      <c r="R81" t="s">
+      <c r="S81" t="s">
         <v>904</v>
       </c>
-      <c r="U81" t="s">
-        <v>1118</v>
+      <c r="V81" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="82">
@@ -8629,254 +8926,265 @@
         <v>15</v>
       </c>
       <c r="Q82" t="s">
+        <v>19</v>
+      </c>
+      <c r="R82" t="s">
         <v>407</v>
       </c>
-      <c r="R82" t="s">
+      <c r="S82" t="s">
         <v>421</v>
       </c>
-      <c r="U82" t="s">
-        <v>1118</v>
+      <c r="V82" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="0" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>1152</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="E83" s="0"/>
-      <c r="F83" s="0">
+      <c r="A83" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F83">
         <v>4</v>
       </c>
-      <c r="G83" s="0" t="s">
-        <v>1155</v>
-      </c>
-      <c r="H83" s="0"/>
-      <c r="I83" s="0" t="s">
-        <v>1156</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>1157</v>
-      </c>
-      <c r="K83" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="L83" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="M83" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="N83" s="0">
+      <c r="G83" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1127</v>
+      </c>
+      <c r="J83" t="s">
+        <v>1128</v>
+      </c>
+      <c r="K83" t="s">
+        <v>1129</v>
+      </c>
+      <c r="L83" t="s">
+        <v>1130</v>
+      </c>
+      <c r="M83" t="s">
+        <v>1131</v>
+      </c>
+      <c r="N83">
         <v>8</v>
       </c>
-      <c r="O83" s="0" t="s">
-        <v>1161</v>
-      </c>
-      <c r="P83" s="0">
+      <c r="O83" t="s">
+        <v>1132</v>
+      </c>
+      <c r="P83">
         <v>30</v>
       </c>
-      <c r="Q83" s="0" t="s">
-        <v>1162</v>
-      </c>
-      <c r="R83" s="0" t="s">
-        <v>1163</v>
-      </c>
-      <c r="S83" s="0" t="s">
-        <v>1164</v>
-      </c>
-      <c r="T83" s="0"/>
-      <c r="U83" s="0"/>
+      <c r="Q83" t="s">
+        <v>19</v>
+      </c>
+      <c r="R83" t="s">
+        <v>1133</v>
+      </c>
+      <c r="S83" t="s">
+        <v>1134</v>
+      </c>
+      <c r="T83" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>1011</v>
+        <v>996</v>
       </c>
       <c r="B84" t="s">
-        <v>1012</v>
+        <v>997</v>
       </c>
       <c r="C84" t="s">
-        <v>1013</v>
+        <v>998</v>
       </c>
       <c r="D84" t="s">
-        <v>1014</v>
+        <v>999</v>
       </c>
       <c r="E84" t="s">
-        <v>1015</v>
+        <v>1000</v>
       </c>
       <c r="F84">
         <v>4</v>
       </c>
       <c r="G84" t="s">
-        <v>1016</v>
+        <v>1001</v>
       </c>
       <c r="H84" t="s">
-        <v>1017</v>
+        <v>1002</v>
       </c>
       <c r="I84" t="s">
-        <v>1018</v>
+        <v>1003</v>
       </c>
       <c r="J84" t="s">
-        <v>1019</v>
+        <v>1004</v>
       </c>
       <c r="K84" t="s">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="L84" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
       <c r="M84" t="s">
-        <v>1022</v>
+        <v>1007</v>
       </c>
       <c r="N84">
         <v>8</v>
       </c>
       <c r="O84" t="s">
-        <v>1023</v>
+        <v>1008</v>
       </c>
       <c r="P84">
         <v>15</v>
       </c>
       <c r="Q84" t="s">
-        <v>1024</v>
+        <v>19</v>
       </c>
       <c r="R84" t="s">
-        <v>1025</v>
-      </c>
-      <c r="U84" t="s">
-        <v>1118</v>
+        <v>1009</v>
+      </c>
+      <c r="S84" t="s">
+        <v>1010</v>
+      </c>
+      <c r="V84" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>1026</v>
+        <v>1011</v>
       </c>
       <c r="B85" t="s">
-        <v>1027</v>
+        <v>1012</v>
       </c>
       <c r="C85" t="s">
-        <v>1028</v>
+        <v>1013</v>
       </c>
       <c r="D85" t="s">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="E85" t="s">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="F85">
         <v>4</v>
       </c>
       <c r="G85" t="s">
-        <v>1031</v>
+        <v>1016</v>
       </c>
       <c r="H85" t="s">
-        <v>1032</v>
+        <v>1017</v>
       </c>
       <c r="I85" t="s">
-        <v>1033</v>
+        <v>1018</v>
       </c>
       <c r="J85" t="s">
-        <v>1034</v>
+        <v>1019</v>
       </c>
       <c r="K85" t="s">
-        <v>1035</v>
+        <v>1020</v>
       </c>
       <c r="L85" t="s">
-        <v>1036</v>
+        <v>1021</v>
       </c>
       <c r="M85" t="s">
-        <v>1037</v>
+        <v>1022</v>
       </c>
       <c r="N85">
         <v>8</v>
       </c>
       <c r="O85" t="s">
-        <v>1038</v>
+        <v>1023</v>
       </c>
       <c r="P85">
         <v>0.2</v>
       </c>
       <c r="Q85" t="s">
-        <v>1039</v>
+        <v>19</v>
       </c>
       <c r="R85" t="s">
-        <v>1040</v>
-      </c>
-      <c r="T85" t="s">
-        <v>1041</v>
+        <v>1024</v>
+      </c>
+      <c r="S85" t="s">
+        <v>1025</v>
       </c>
       <c r="U85" t="s">
-        <v>1149</v>
+        <v>1026</v>
+      </c>
+      <c r="V85" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>1101</v>
+        <v>1086</v>
       </c>
       <c r="B86" t="s">
-        <v>1102</v>
+        <v>1087</v>
       </c>
       <c r="C86" t="s">
-        <v>1103</v>
+        <v>1088</v>
       </c>
       <c r="D86" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="F86">
         <v>4</v>
       </c>
       <c r="G86" t="s">
-        <v>1105</v>
+        <v>1090</v>
       </c>
       <c r="H86" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="I86" t="s">
-        <v>1107</v>
+        <v>1092</v>
       </c>
       <c r="J86" t="s">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="K86" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="L86" t="s">
-        <v>1110</v>
+        <v>1095</v>
       </c>
       <c r="M86" t="s">
-        <v>1111</v>
+        <v>1096</v>
       </c>
       <c r="N86">
         <v>8</v>
       </c>
       <c r="O86" t="s">
-        <v>1112</v>
+        <v>1097</v>
       </c>
       <c r="P86">
         <v>1</v>
       </c>
       <c r="Q86" t="s">
-        <v>1113</v>
+        <v>19</v>
       </c>
       <c r="R86" t="s">
-        <v>1114</v>
-      </c>
-      <c r="T86" t="s">
-        <v>1115</v>
+        <v>1098</v>
+      </c>
+      <c r="S86" t="s">
+        <v>1099</v>
       </c>
       <c r="U86" t="s">
-        <v>1149</v>
+        <v>1100</v>
+      </c>
+      <c r="V86" t="s">
+        <v>1120</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:T83">
+  <sortState ref="A2:U83">
     <sortCondition ref="A2:A83"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>